<commit_message>
Verify that bathtubs are properly loaded and visible within the application
Adds a script to check if the 'Bathtubs' sheet exists in the Excel data source.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/d7bbe0b5-cd96-4ae5-83fc-a3e102de8a6c.jpg
</commit_message>
<xml_diff>
--- a/data/Product Data.xlsx
+++ b/data/Product Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/PythonScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="11_8E13AE15F5EA82F19A54427495912BA654E97DEA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90E5C4A5-91BC-4751-A91A-6FFEB2C37C1F}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_8E13AE15F5EA82F19A54427495912BA654E97DEA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4F6BDD-0A2B-461A-90B5-689B75C2BB47}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shower Bases" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bathtubs!$A$1:$M$237</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Enclosures!$A$1:$L$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Enclosures!$A$1:$K$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Return Panels'!$A$1:$F$33</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Screens!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Shower Doors'!$A$1:$O$219</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Screens!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Shower Doors'!$A$1:$N$219</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Showers!$A$1:$I$151</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Tub Doors'!$A$1:$J$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Tub Doors'!$A$1:$I$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Tub Showers'!$A$1:$H$105</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Walls!$A$1:$L$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Walls!$A$1:$K$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7338" uniqueCount="1802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7062" uniqueCount="1764">
   <si>
     <t>Unique ID</t>
   </si>
@@ -5345,120 +5345,6 @@
   </si>
   <si>
     <t>6mm</t>
-  </si>
-  <si>
-    <t>Ranking</t>
-  </si>
-  <si>
-    <t>1550</t>
-  </si>
-  <si>
-    <t>1025</t>
-  </si>
-  <si>
-    <t>1850</t>
-  </si>
-  <si>
-    <t>1250</t>
-  </si>
-  <si>
-    <t>1750</t>
-  </si>
-  <si>
-    <t>1050</t>
-  </si>
-  <si>
-    <t>2650</t>
-  </si>
-  <si>
-    <t>3250</t>
-  </si>
-  <si>
-    <t>3750</t>
-  </si>
-  <si>
-    <t>3550</t>
-  </si>
-  <si>
-    <t>1150</t>
-  </si>
-  <si>
-    <t>2350</t>
-  </si>
-  <si>
-    <t>1950</t>
-  </si>
-  <si>
-    <t>3150</t>
-  </si>
-  <si>
-    <t>1400</t>
-  </si>
-  <si>
-    <t>3850</t>
-  </si>
-  <si>
-    <t>2850</t>
-  </si>
-  <si>
-    <t>1350</t>
-  </si>
-  <si>
-    <t>3050</t>
-  </si>
-  <si>
-    <t>2750</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>2150</t>
-  </si>
-  <si>
-    <t>2950</t>
-  </si>
-  <si>
-    <t>2250</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>3350</t>
-  </si>
-  <si>
-    <t>1725</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>1450</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>3650</t>
-  </si>
-  <si>
-    <t>2050</t>
-  </si>
-  <si>
-    <t>3950</t>
-  </si>
-  <si>
-    <t>1410</t>
-  </si>
-  <si>
-    <t>210</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>160</t>
   </si>
 </sst>
 </file>
@@ -20505,10 +20391,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20523,12 +20409,11 @@
     <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -20562,11 +20447,8 @@
       <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>936</v>
       </c>
@@ -20600,11 +20482,8 @@
       <c r="K2" t="s">
         <v>942</v>
       </c>
-      <c r="L2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>189</v>
       </c>
@@ -20638,11 +20517,8 @@
       <c r="K3" t="s">
         <v>942</v>
       </c>
-      <c r="L3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>945</v>
       </c>
@@ -20676,11 +20552,8 @@
       <c r="K4" t="s">
         <v>942</v>
       </c>
-      <c r="L4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>948</v>
       </c>
@@ -20714,11 +20587,8 @@
       <c r="K5" t="s">
         <v>942</v>
       </c>
-      <c r="L5">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>949</v>
       </c>
@@ -20752,11 +20622,8 @@
       <c r="K6" t="s">
         <v>953</v>
       </c>
-      <c r="L6">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>954</v>
       </c>
@@ -20790,11 +20657,8 @@
       <c r="K7" t="s">
         <v>942</v>
       </c>
-      <c r="L7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>192</v>
       </c>
@@ -20828,11 +20692,8 @@
       <c r="K8" t="s">
         <v>942</v>
       </c>
-      <c r="L8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>955</v>
       </c>
@@ -20866,11 +20727,8 @@
       <c r="K9" t="s">
         <v>958</v>
       </c>
-      <c r="L9">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>959</v>
       </c>
@@ -20904,11 +20762,8 @@
       <c r="K10" t="s">
         <v>958</v>
       </c>
-      <c r="L10">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -20942,11 +20797,8 @@
       <c r="K11" t="s">
         <v>942</v>
       </c>
-      <c r="L11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -20980,11 +20832,8 @@
       <c r="K12" t="s">
         <v>942</v>
       </c>
-      <c r="L12">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>963</v>
       </c>
@@ -21018,11 +20867,8 @@
       <c r="K13" t="s">
         <v>965</v>
       </c>
-      <c r="L13">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>966</v>
       </c>
@@ -21056,11 +20902,8 @@
       <c r="K14" t="s">
         <v>942</v>
       </c>
-      <c r="L14">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -21094,11 +20937,8 @@
       <c r="K15" t="s">
         <v>942</v>
       </c>
-      <c r="L15">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>967</v>
       </c>
@@ -21132,11 +20972,8 @@
       <c r="K16" t="s">
         <v>970</v>
       </c>
-      <c r="L16">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>971</v>
       </c>
@@ -21170,11 +21007,8 @@
       <c r="K17" t="s">
         <v>942</v>
       </c>
-      <c r="L17">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>972</v>
       </c>
@@ -21208,11 +21042,8 @@
       <c r="K18" t="s">
         <v>953</v>
       </c>
-      <c r="L18">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>974</v>
       </c>
@@ -21246,11 +21077,8 @@
       <c r="K19" t="s">
         <v>942</v>
       </c>
-      <c r="L19">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>975</v>
       </c>
@@ -21284,11 +21112,8 @@
       <c r="K20" t="s">
         <v>942</v>
       </c>
-      <c r="L20">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>977</v>
       </c>
@@ -21322,11 +21147,8 @@
       <c r="K21" t="s">
         <v>942</v>
       </c>
-      <c r="L21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>978</v>
       </c>
@@ -21360,11 +21182,8 @@
       <c r="K22" t="s">
         <v>970</v>
       </c>
-      <c r="L22">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>980</v>
       </c>
@@ -21398,11 +21217,8 @@
       <c r="K23" t="s">
         <v>953</v>
       </c>
-      <c r="L23">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>982</v>
       </c>
@@ -21436,11 +21252,8 @@
       <c r="K24" t="s">
         <v>970</v>
       </c>
-      <c r="L24">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>984</v>
       </c>
@@ -21474,11 +21287,8 @@
       <c r="K25" t="s">
         <v>942</v>
       </c>
-      <c r="L25">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>986</v>
       </c>
@@ -21512,11 +21322,8 @@
       <c r="K26" t="s">
         <v>953</v>
       </c>
-      <c r="L26">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>988</v>
       </c>
@@ -21550,11 +21357,8 @@
       <c r="K27" t="s">
         <v>990</v>
       </c>
-      <c r="L27">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>991</v>
       </c>
@@ -21588,11 +21392,8 @@
       <c r="K28" t="s">
         <v>990</v>
       </c>
-      <c r="L28">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>993</v>
       </c>
@@ -21626,11 +21427,8 @@
       <c r="K29" t="s">
         <v>942</v>
       </c>
-      <c r="L29">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>994</v>
       </c>
@@ -21664,11 +21462,8 @@
       <c r="K30" t="s">
         <v>942</v>
       </c>
-      <c r="L30">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>995</v>
       </c>
@@ -21702,11 +21497,8 @@
       <c r="K31" t="s">
         <v>970</v>
       </c>
-      <c r="L31">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>997</v>
       </c>
@@ -21740,11 +21532,8 @@
       <c r="K32" t="s">
         <v>965</v>
       </c>
-      <c r="L32">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>999</v>
       </c>
@@ -21778,11 +21567,8 @@
       <c r="K33" t="s">
         <v>942</v>
       </c>
-      <c r="L33">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1000</v>
       </c>
@@ -21816,22 +21602,19 @@
       <c r="K34" t="s">
         <v>942</v>
       </c>
-      <c r="L34">
-        <v>1000</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L34" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <autoFilter ref="A1:K34" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21847,7 +21630,7 @@
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -21869,12 +21652,9 @@
       <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>1764</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0500-000000000000}"/>
+  <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21882,10 +21662,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:O219"/>
+  <dimension ref="A1:N219"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21902,11 +21682,10 @@
     <col min="11" max="11" width="14.44140625" customWidth="1"/>
     <col min="12" max="12" width="25.6640625" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" customWidth="1"/>
-    <col min="15" max="15" width="35.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.21875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -21946,14 +21725,11 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
-        <v>1764</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>1007</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1008</v>
       </c>
@@ -21990,11 +21766,8 @@
       <c r="M2" t="s">
         <v>1010</v>
       </c>
-      <c r="N2" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1011</v>
       </c>
@@ -22031,11 +21804,8 @@
       <c r="M3" t="s">
         <v>1015</v>
       </c>
-      <c r="N3" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1016</v>
       </c>
@@ -22072,11 +21842,8 @@
       <c r="M4" t="s">
         <v>1020</v>
       </c>
-      <c r="N4" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1021</v>
       </c>
@@ -22113,11 +21880,8 @@
       <c r="M5" t="s">
         <v>1024</v>
       </c>
-      <c r="N5" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1025</v>
       </c>
@@ -22154,11 +21918,8 @@
       <c r="M6" t="s">
         <v>1027</v>
       </c>
-      <c r="N6" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1028</v>
       </c>
@@ -22195,11 +21956,8 @@
       <c r="M7" t="s">
         <v>1033</v>
       </c>
-      <c r="N7" t="s">
-        <v>1785</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1034</v>
       </c>
@@ -22236,11 +21994,8 @@
       <c r="M8" t="s">
         <v>1038</v>
       </c>
-      <c r="N8" t="s">
-        <v>1786</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1039</v>
       </c>
@@ -22277,11 +22032,8 @@
       <c r="M9" t="s">
         <v>1041</v>
       </c>
-      <c r="N9" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1042</v>
       </c>
@@ -22318,11 +22070,8 @@
       <c r="M10" t="s">
         <v>1046</v>
       </c>
-      <c r="N10" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1047</v>
       </c>
@@ -22359,11 +22108,8 @@
       <c r="M11" t="s">
         <v>1049</v>
       </c>
-      <c r="N11" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1050</v>
       </c>
@@ -22400,11 +22146,8 @@
       <c r="M12" t="s">
         <v>1052</v>
       </c>
-      <c r="N12" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1053</v>
       </c>
@@ -22441,11 +22184,8 @@
       <c r="M13" t="s">
         <v>1041</v>
       </c>
-      <c r="N13" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1056</v>
       </c>
@@ -22482,11 +22222,8 @@
       <c r="M14" t="s">
         <v>1058</v>
       </c>
-      <c r="N14" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1059</v>
       </c>
@@ -22523,11 +22260,8 @@
       <c r="M15" t="s">
         <v>1020</v>
       </c>
-      <c r="N15" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1062</v>
       </c>
@@ -22564,11 +22298,8 @@
       <c r="M16" t="s">
         <v>1064</v>
       </c>
-      <c r="N16" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1065</v>
       </c>
@@ -22605,11 +22336,8 @@
       <c r="M17" t="s">
         <v>1067</v>
       </c>
-      <c r="N17" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1068</v>
       </c>
@@ -22646,11 +22374,8 @@
       <c r="M18" t="s">
         <v>1071</v>
       </c>
-      <c r="N18" t="s">
-        <v>1789</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1072</v>
       </c>
@@ -22687,11 +22412,8 @@
       <c r="M19" t="s">
         <v>1075</v>
       </c>
-      <c r="N19" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1076</v>
       </c>
@@ -22728,11 +22450,8 @@
       <c r="M20" t="s">
         <v>1078</v>
       </c>
-      <c r="N20" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1079</v>
       </c>
@@ -22769,11 +22488,8 @@
       <c r="M21" t="s">
         <v>1081</v>
       </c>
-      <c r="N21" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1082</v>
       </c>
@@ -22810,11 +22526,8 @@
       <c r="M22" t="s">
         <v>1024</v>
       </c>
-      <c r="N22" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1084</v>
       </c>
@@ -22851,11 +22564,8 @@
       <c r="M23" t="s">
         <v>1086</v>
       </c>
-      <c r="N23" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1087</v>
       </c>
@@ -22892,11 +22602,8 @@
       <c r="M24" t="s">
         <v>1089</v>
       </c>
-      <c r="N24" t="s">
-        <v>1791</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1090</v>
       </c>
@@ -22933,11 +22640,8 @@
       <c r="M25" t="s">
         <v>1094</v>
       </c>
-      <c r="N25" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1095</v>
       </c>
@@ -22974,11 +22678,8 @@
       <c r="M26" t="s">
         <v>1097</v>
       </c>
-      <c r="N26" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1098</v>
       </c>
@@ -23015,11 +22716,8 @@
       <c r="M27" t="s">
         <v>1015</v>
       </c>
-      <c r="N27" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1100</v>
       </c>
@@ -23056,11 +22754,8 @@
       <c r="M28" t="s">
         <v>1081</v>
       </c>
-      <c r="N28" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1103</v>
       </c>
@@ -23097,11 +22792,8 @@
       <c r="M29" t="s">
         <v>1067</v>
       </c>
-      <c r="N29" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1107</v>
       </c>
@@ -23138,11 +22830,8 @@
       <c r="M30" t="s">
         <v>1041</v>
       </c>
-      <c r="N30" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1109</v>
       </c>
@@ -23179,11 +22868,8 @@
       <c r="M31" t="s">
         <v>1113</v>
       </c>
-      <c r="N31" t="s">
-        <v>1792</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1114</v>
       </c>
@@ -23220,11 +22906,8 @@
       <c r="M32" t="s">
         <v>1116</v>
       </c>
-      <c r="N32" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1117</v>
       </c>
@@ -23261,11 +22944,8 @@
       <c r="M33" t="s">
         <v>1119</v>
       </c>
-      <c r="N33" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1120</v>
       </c>
@@ -23302,11 +22982,8 @@
       <c r="M34" t="s">
         <v>1041</v>
       </c>
-      <c r="N34" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1122</v>
       </c>
@@ -23343,11 +23020,8 @@
       <c r="M35" t="s">
         <v>1124</v>
       </c>
-      <c r="N35" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1125</v>
       </c>
@@ -23384,11 +23058,8 @@
       <c r="M36" t="s">
         <v>1038</v>
       </c>
-      <c r="N36" t="s">
-        <v>1786</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1127</v>
       </c>
@@ -23425,11 +23096,8 @@
       <c r="M37" t="s">
         <v>1129</v>
       </c>
-      <c r="N37" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1130</v>
       </c>
@@ -23466,11 +23134,8 @@
       <c r="M38" t="s">
         <v>1064</v>
       </c>
-      <c r="N38" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1132</v>
       </c>
@@ -23507,11 +23172,8 @@
       <c r="M39" t="s">
         <v>1134</v>
       </c>
-      <c r="N39" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1135</v>
       </c>
@@ -23548,11 +23210,8 @@
       <c r="M40" t="s">
         <v>1138</v>
       </c>
-      <c r="N40" t="s">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1139</v>
       </c>
@@ -23589,11 +23248,8 @@
       <c r="M41" t="s">
         <v>1141</v>
       </c>
-      <c r="N41" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1142</v>
       </c>
@@ -23630,11 +23286,8 @@
       <c r="M42" t="s">
         <v>1041</v>
       </c>
-      <c r="N42" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1144</v>
       </c>
@@ -23671,11 +23324,8 @@
       <c r="M43" t="s">
         <v>1041</v>
       </c>
-      <c r="N43" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1147</v>
       </c>
@@ -23712,11 +23362,8 @@
       <c r="M44" t="s">
         <v>1020</v>
       </c>
-      <c r="N44" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1149</v>
       </c>
@@ -23753,11 +23400,8 @@
       <c r="M45" t="s">
         <v>1152</v>
       </c>
-      <c r="N45" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1153</v>
       </c>
@@ -23794,11 +23438,8 @@
       <c r="M46" t="s">
         <v>1155</v>
       </c>
-      <c r="N46" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1156</v>
       </c>
@@ -23835,11 +23476,8 @@
       <c r="M47" t="s">
         <v>1015</v>
       </c>
-      <c r="N47" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1158</v>
       </c>
@@ -23876,11 +23514,8 @@
       <c r="M48" t="s">
         <v>1075</v>
       </c>
-      <c r="N48" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>1161</v>
       </c>
@@ -23917,11 +23552,8 @@
       <c r="M49" t="s">
         <v>1075</v>
       </c>
-      <c r="N49" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>1164</v>
       </c>
@@ -23958,11 +23590,8 @@
       <c r="M50" t="s">
         <v>1119</v>
       </c>
-      <c r="N50" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>1166</v>
       </c>
@@ -23999,11 +23628,8 @@
       <c r="M51" t="s">
         <v>1152</v>
       </c>
-      <c r="N51" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>1170</v>
       </c>
@@ -24040,11 +23666,8 @@
       <c r="M52" t="s">
         <v>1027</v>
       </c>
-      <c r="N52" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>1172</v>
       </c>
@@ -24081,11 +23704,8 @@
       <c r="M53" t="s">
         <v>1174</v>
       </c>
-      <c r="N53" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>1175</v>
       </c>
@@ -24122,11 +23742,8 @@
       <c r="M54" t="s">
         <v>1020</v>
       </c>
-      <c r="N54" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>1177</v>
       </c>
@@ -24163,11 +23780,8 @@
       <c r="M55" t="s">
         <v>1152</v>
       </c>
-      <c r="N55" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>1180</v>
       </c>
@@ -24204,11 +23818,8 @@
       <c r="M56" t="s">
         <v>1119</v>
       </c>
-      <c r="N56" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>1182</v>
       </c>
@@ -24245,11 +23856,8 @@
       <c r="M57" t="s">
         <v>1075</v>
       </c>
-      <c r="N57" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>1185</v>
       </c>
@@ -24286,11 +23894,8 @@
       <c r="M58" t="s">
         <v>1152</v>
       </c>
-      <c r="N58" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>1188</v>
       </c>
@@ -24327,11 +23932,8 @@
       <c r="M59" t="s">
         <v>1152</v>
       </c>
-      <c r="N59" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>1190</v>
       </c>
@@ -24368,11 +23970,8 @@
       <c r="M60" t="s">
         <v>1152</v>
       </c>
-      <c r="N60" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>1192</v>
       </c>
@@ -24409,11 +24008,8 @@
       <c r="M61" t="s">
         <v>1194</v>
       </c>
-      <c r="N61" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>1195</v>
       </c>
@@ -24450,11 +24046,8 @@
       <c r="M62" t="s">
         <v>1094</v>
       </c>
-      <c r="N62" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>1197</v>
       </c>
@@ -24491,11 +24084,8 @@
       <c r="M63" t="s">
         <v>1141</v>
       </c>
-      <c r="N63" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>1199</v>
       </c>
@@ -24532,11 +24122,8 @@
       <c r="M64" t="s">
         <v>1020</v>
       </c>
-      <c r="N64" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1201</v>
       </c>
@@ -24573,11 +24160,8 @@
       <c r="M65" t="s">
         <v>1027</v>
       </c>
-      <c r="N65" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1203</v>
       </c>
@@ -24614,11 +24198,8 @@
       <c r="M66" t="s">
         <v>1205</v>
       </c>
-      <c r="N66" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1206</v>
       </c>
@@ -24655,11 +24236,8 @@
       <c r="M67" t="s">
         <v>1152</v>
       </c>
-      <c r="N67" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1209</v>
       </c>
@@ -24696,11 +24274,8 @@
       <c r="M68" t="s">
         <v>1086</v>
       </c>
-      <c r="N68" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1212</v>
       </c>
@@ -24737,11 +24312,8 @@
       <c r="M69" t="s">
         <v>1152</v>
       </c>
-      <c r="N69" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>1214</v>
       </c>
@@ -24778,11 +24350,8 @@
       <c r="M70" t="s">
         <v>1216</v>
       </c>
-      <c r="N70" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>1217</v>
       </c>
@@ -24819,11 +24388,8 @@
       <c r="M71" t="s">
         <v>1219</v>
       </c>
-      <c r="N71" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>1220</v>
       </c>
@@ -24860,11 +24426,8 @@
       <c r="M72" t="s">
         <v>1152</v>
       </c>
-      <c r="N72" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>1222</v>
       </c>
@@ -24901,11 +24464,8 @@
       <c r="M73" t="s">
         <v>1067</v>
       </c>
-      <c r="N73" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>1224</v>
       </c>
@@ -24942,11 +24502,8 @@
       <c r="M74" t="s">
         <v>1226</v>
       </c>
-      <c r="N74" t="s">
-        <v>1795</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>1227</v>
       </c>
@@ -24983,11 +24540,8 @@
       <c r="M75" t="s">
         <v>1119</v>
       </c>
-      <c r="N75" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>1229</v>
       </c>
@@ -25024,11 +24578,8 @@
       <c r="M76" t="s">
         <v>1194</v>
       </c>
-      <c r="N76" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>1232</v>
       </c>
@@ -25065,11 +24616,8 @@
       <c r="M77" t="s">
         <v>1078</v>
       </c>
-      <c r="N77" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>1234</v>
       </c>
@@ -25106,11 +24654,8 @@
       <c r="M78" t="s">
         <v>1020</v>
       </c>
-      <c r="N78" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1237</v>
       </c>
@@ -25147,11 +24692,8 @@
       <c r="M79" t="s">
         <v>1241</v>
       </c>
-      <c r="N79" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>1242</v>
       </c>
@@ -25188,11 +24730,8 @@
       <c r="M80" t="s">
         <v>1244</v>
       </c>
-      <c r="N80" t="s">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>1245</v>
       </c>
@@ -25229,11 +24768,8 @@
       <c r="M81" t="s">
         <v>1067</v>
       </c>
-      <c r="N81" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>1247</v>
       </c>
@@ -25270,11 +24806,8 @@
       <c r="M82" t="s">
         <v>1250</v>
       </c>
-      <c r="N82" t="s">
-        <v>1797</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>1251</v>
       </c>
@@ -25305,11 +24838,8 @@
       <c r="M83" t="s">
         <v>1253</v>
       </c>
-      <c r="N83" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>1254</v>
       </c>
@@ -25346,11 +24876,8 @@
       <c r="M84" t="s">
         <v>1257</v>
       </c>
-      <c r="N84" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>1258</v>
       </c>
@@ -25387,11 +24914,8 @@
       <c r="M85" t="s">
         <v>1020</v>
       </c>
-      <c r="N85" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>1260</v>
       </c>
@@ -25428,11 +24952,8 @@
       <c r="M86" t="s">
         <v>1262</v>
       </c>
-      <c r="N86">
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>1263</v>
       </c>
@@ -25469,11 +24990,8 @@
       <c r="M87" t="s">
         <v>1067</v>
       </c>
-      <c r="N87" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>1265</v>
       </c>
@@ -25510,11 +25028,8 @@
       <c r="M88" t="s">
         <v>1067</v>
       </c>
-      <c r="N88" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>1267</v>
       </c>
@@ -25551,11 +25066,8 @@
       <c r="M89" t="s">
         <v>1244</v>
       </c>
-      <c r="N89" t="s">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>1269</v>
       </c>
@@ -25592,11 +25104,8 @@
       <c r="M90" t="s">
         <v>1075</v>
       </c>
-      <c r="N90" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>1272</v>
       </c>
@@ -25633,11 +25142,8 @@
       <c r="M91" t="s">
         <v>1097</v>
       </c>
-      <c r="N91" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>1274</v>
       </c>
@@ -25674,11 +25180,8 @@
       <c r="M92" t="s">
         <v>1081</v>
       </c>
-      <c r="N92" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>1276</v>
       </c>
@@ -25715,11 +25218,8 @@
       <c r="M93" t="s">
         <v>1155</v>
       </c>
-      <c r="N93" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>1278</v>
       </c>
@@ -25756,11 +25256,8 @@
       <c r="M94" t="s">
         <v>1152</v>
       </c>
-      <c r="N94" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>1280</v>
       </c>
@@ -25797,11 +25294,8 @@
       <c r="M95" t="s">
         <v>1119</v>
       </c>
-      <c r="N95" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>1281</v>
       </c>
@@ -25838,11 +25332,8 @@
       <c r="M96" t="s">
         <v>1124</v>
       </c>
-      <c r="N96" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>1283</v>
       </c>
@@ -25879,11 +25370,8 @@
       <c r="M97" t="s">
         <v>1285</v>
       </c>
-      <c r="N97" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>1286</v>
       </c>
@@ -25920,11 +25408,8 @@
       <c r="M98" t="s">
         <v>1058</v>
       </c>
-      <c r="N98" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>1288</v>
       </c>
@@ -25961,11 +25446,8 @@
       <c r="M99" t="s">
         <v>1067</v>
       </c>
-      <c r="N99" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>1290</v>
       </c>
@@ -26002,11 +25484,8 @@
       <c r="M100" t="s">
         <v>1285</v>
       </c>
-      <c r="N100" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>1292</v>
       </c>
@@ -26043,11 +25522,8 @@
       <c r="M101" t="s">
         <v>1119</v>
       </c>
-      <c r="N101" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>1293</v>
       </c>
@@ -26084,11 +25560,8 @@
       <c r="M102" t="s">
         <v>1219</v>
       </c>
-      <c r="N102" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>1295</v>
       </c>
@@ -26125,11 +25598,8 @@
       <c r="M103" t="s">
         <v>1067</v>
       </c>
-      <c r="N103" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>1298</v>
       </c>
@@ -26166,11 +25636,8 @@
       <c r="M104" t="s">
         <v>1086</v>
       </c>
-      <c r="N104" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>1300</v>
       </c>
@@ -26207,11 +25674,8 @@
       <c r="M105" t="s">
         <v>1046</v>
       </c>
-      <c r="N105" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>1302</v>
       </c>
@@ -26248,11 +25712,8 @@
       <c r="M106" t="s">
         <v>1033</v>
       </c>
-      <c r="N106" t="s">
-        <v>1785</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>1305</v>
       </c>
@@ -26289,11 +25750,8 @@
       <c r="M107" t="s">
         <v>1152</v>
       </c>
-      <c r="N107" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>1307</v>
       </c>
@@ -26330,11 +25788,8 @@
       <c r="M108" t="s">
         <v>1041</v>
       </c>
-      <c r="N108" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>1309</v>
       </c>
@@ -26371,11 +25826,8 @@
       <c r="M109" t="s">
         <v>1052</v>
       </c>
-      <c r="N109" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>1311</v>
       </c>
@@ -26412,11 +25864,8 @@
       <c r="M110" t="s">
         <v>1134</v>
       </c>
-      <c r="N110" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>1313</v>
       </c>
@@ -26453,11 +25902,8 @@
       <c r="M111" t="s">
         <v>1027</v>
       </c>
-      <c r="N111" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>1315</v>
       </c>
@@ -26494,11 +25940,8 @@
       <c r="M112" t="s">
         <v>1194</v>
       </c>
-      <c r="N112" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>1319</v>
       </c>
@@ -26535,11 +25978,8 @@
       <c r="M113" t="s">
         <v>1152</v>
       </c>
-      <c r="N113" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>1322</v>
       </c>
@@ -26576,11 +26016,8 @@
       <c r="M114" t="s">
         <v>1124</v>
       </c>
-      <c r="N114" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>1324</v>
       </c>
@@ -26617,11 +26054,8 @@
       <c r="M115" t="s">
         <v>1253</v>
       </c>
-      <c r="N115" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>1326</v>
       </c>
@@ -26658,11 +26092,8 @@
       <c r="M116" t="s">
         <v>1328</v>
       </c>
-      <c r="N116" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>1329</v>
       </c>
@@ -26699,11 +26130,8 @@
       <c r="M117" t="s">
         <v>1081</v>
       </c>
-      <c r="N117" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>1331</v>
       </c>
@@ -26740,11 +26168,8 @@
       <c r="M118" t="s">
         <v>1041</v>
       </c>
-      <c r="N118" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>1334</v>
       </c>
@@ -26781,11 +26206,8 @@
       <c r="M119" t="s">
         <v>1129</v>
       </c>
-      <c r="N119" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>1336</v>
       </c>
@@ -26822,11 +26244,8 @@
       <c r="M120" t="s">
         <v>1205</v>
       </c>
-      <c r="N120" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>1338</v>
       </c>
@@ -26863,11 +26282,8 @@
       <c r="M121" t="s">
         <v>1340</v>
       </c>
-      <c r="N121" t="s">
-        <v>1798</v>
-      </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>1341</v>
       </c>
@@ -26904,11 +26320,8 @@
       <c r="M122" t="s">
         <v>1129</v>
       </c>
-      <c r="N122" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>1343</v>
       </c>
@@ -26945,11 +26358,8 @@
       <c r="M123" t="s">
         <v>1041</v>
       </c>
-      <c r="N123" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>1345</v>
       </c>
@@ -26986,11 +26396,8 @@
       <c r="M124" t="s">
         <v>1094</v>
       </c>
-      <c r="N124" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>1347</v>
       </c>
@@ -27027,11 +26434,8 @@
       <c r="M125" t="s">
         <v>1027</v>
       </c>
-      <c r="N125" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>1349</v>
       </c>
@@ -27068,11 +26472,8 @@
       <c r="M126" t="s">
         <v>1094</v>
       </c>
-      <c r="N126" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>1351</v>
       </c>
@@ -27109,11 +26510,8 @@
       <c r="M127" t="s">
         <v>1027</v>
       </c>
-      <c r="N127" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>1352</v>
       </c>
@@ -27150,11 +26548,8 @@
       <c r="M128" t="s">
         <v>1049</v>
       </c>
-      <c r="N128" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>1354</v>
       </c>
@@ -27191,11 +26586,8 @@
       <c r="M129" t="s">
         <v>1058</v>
       </c>
-      <c r="N129" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>1356</v>
       </c>
@@ -27232,11 +26624,8 @@
       <c r="M130" t="s">
         <v>1058</v>
       </c>
-      <c r="N130" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>1358</v>
       </c>
@@ -27273,11 +26662,8 @@
       <c r="M131" t="s">
         <v>1361</v>
       </c>
-      <c r="N131" t="s">
-        <v>1799</v>
-      </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>1362</v>
       </c>
@@ -27314,11 +26700,8 @@
       <c r="M132" t="s">
         <v>1038</v>
       </c>
-      <c r="N132" t="s">
-        <v>1786</v>
-      </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>1364</v>
       </c>
@@ -27355,11 +26738,8 @@
       <c r="M133" t="s">
         <v>1067</v>
       </c>
-      <c r="N133" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>1366</v>
       </c>
@@ -27396,11 +26776,8 @@
       <c r="M134" t="s">
         <v>1129</v>
       </c>
-      <c r="N134" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>1369</v>
       </c>
@@ -27437,11 +26814,8 @@
       <c r="M135" t="s">
         <v>1086</v>
       </c>
-      <c r="N135" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>1373</v>
       </c>
@@ -27478,11 +26852,8 @@
       <c r="M136" t="s">
         <v>1375</v>
       </c>
-      <c r="N136" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>1376</v>
       </c>
@@ -27519,11 +26890,8 @@
       <c r="M137" t="s">
         <v>1340</v>
       </c>
-      <c r="N137" t="s">
-        <v>1798</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>1378</v>
       </c>
@@ -27560,11 +26928,8 @@
       <c r="M138" t="s">
         <v>1078</v>
       </c>
-      <c r="N138" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>1380</v>
       </c>
@@ -27601,11 +26966,8 @@
       <c r="M139" t="s">
         <v>1097</v>
       </c>
-      <c r="N139" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>1382</v>
       </c>
@@ -27642,11 +27004,8 @@
       <c r="M140" t="s">
         <v>1138</v>
       </c>
-      <c r="N140" t="s">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>1384</v>
       </c>
@@ -27683,11 +27042,8 @@
       <c r="M141" t="s">
         <v>1067</v>
       </c>
-      <c r="N141" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>1387</v>
       </c>
@@ -27724,11 +27080,8 @@
       <c r="M142" t="s">
         <v>1129</v>
       </c>
-      <c r="N142" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>1389</v>
       </c>
@@ -27765,11 +27118,8 @@
       <c r="M143" t="s">
         <v>1097</v>
       </c>
-      <c r="N143" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>1391</v>
       </c>
@@ -27806,11 +27156,8 @@
       <c r="M144" t="s">
         <v>1152</v>
       </c>
-      <c r="N144" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>1394</v>
       </c>
@@ -27847,11 +27194,8 @@
       <c r="M145" t="s">
         <v>1086</v>
       </c>
-      <c r="N145" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>1397</v>
       </c>
@@ -27888,11 +27232,8 @@
       <c r="M146" t="s">
         <v>1399</v>
       </c>
-      <c r="N146" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>1400</v>
       </c>
@@ -27929,11 +27270,8 @@
       <c r="M147" t="s">
         <v>1075</v>
       </c>
-      <c r="N147" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>1402</v>
       </c>
@@ -27970,11 +27308,8 @@
       <c r="M148" t="s">
         <v>1216</v>
       </c>
-      <c r="N148" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>1404</v>
       </c>
@@ -28011,11 +27346,8 @@
       <c r="M149" t="s">
         <v>1241</v>
       </c>
-      <c r="N149" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>1407</v>
       </c>
@@ -28052,11 +27384,8 @@
       <c r="M150" t="s">
         <v>1409</v>
       </c>
-      <c r="N150" t="s">
-        <v>1801</v>
-      </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>1410</v>
       </c>
@@ -28093,11 +27422,8 @@
       <c r="M151" t="s">
         <v>1155</v>
       </c>
-      <c r="N151" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>1412</v>
       </c>
@@ -28134,11 +27460,8 @@
       <c r="M152" t="s">
         <v>1058</v>
       </c>
-      <c r="N152" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>1414</v>
       </c>
@@ -28175,11 +27498,8 @@
       <c r="M153" t="s">
         <v>1015</v>
       </c>
-      <c r="N153" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>1416</v>
       </c>
@@ -28216,11 +27536,8 @@
       <c r="M154" t="s">
         <v>1067</v>
       </c>
-      <c r="N154" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>1418</v>
       </c>
@@ -28257,11 +27574,8 @@
       <c r="M155" t="s">
         <v>1420</v>
       </c>
-      <c r="N155" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>1421</v>
       </c>
@@ -28298,11 +27612,8 @@
       <c r="M156" t="s">
         <v>1138</v>
       </c>
-      <c r="N156" t="s">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>1423</v>
       </c>
@@ -28339,11 +27650,8 @@
       <c r="M157" t="s">
         <v>1046</v>
       </c>
-      <c r="N157" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>1425</v>
       </c>
@@ -28380,11 +27688,8 @@
       <c r="M158" t="s">
         <v>1041</v>
       </c>
-      <c r="N158" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>1427</v>
       </c>
@@ -28421,11 +27726,8 @@
       <c r="M159" t="s">
         <v>1046</v>
       </c>
-      <c r="N159" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>1429</v>
       </c>
@@ -28462,11 +27764,8 @@
       <c r="M160" t="s">
         <v>1226</v>
       </c>
-      <c r="N160" t="s">
-        <v>1795</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>1431</v>
       </c>
@@ -28503,11 +27802,8 @@
       <c r="M161" t="s">
         <v>1067</v>
       </c>
-      <c r="N161" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>1433</v>
       </c>
@@ -28544,11 +27840,8 @@
       <c r="M162" t="s">
         <v>1081</v>
       </c>
-      <c r="N162" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>1435</v>
       </c>
@@ -28585,11 +27878,8 @@
       <c r="M163" t="s">
         <v>1116</v>
       </c>
-      <c r="N163" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>1437</v>
       </c>
@@ -28626,11 +27916,8 @@
       <c r="M164" t="s">
         <v>1152</v>
       </c>
-      <c r="N164" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>1439</v>
       </c>
@@ -28667,11 +27954,8 @@
       <c r="M165" t="s">
         <v>1152</v>
       </c>
-      <c r="N165" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>1441</v>
       </c>
@@ -28708,11 +27992,8 @@
       <c r="M166" t="s">
         <v>1138</v>
       </c>
-      <c r="N166" t="s">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>1443</v>
       </c>
@@ -28749,11 +28030,8 @@
       <c r="M167" t="s">
         <v>1027</v>
       </c>
-      <c r="N167" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>1445</v>
       </c>
@@ -28790,11 +28068,8 @@
       <c r="M168" t="s">
         <v>1328</v>
       </c>
-      <c r="N168" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>1447</v>
       </c>
@@ -28831,11 +28106,8 @@
       <c r="M169" t="s">
         <v>1152</v>
       </c>
-      <c r="N169" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>1449</v>
       </c>
@@ -28872,11 +28144,8 @@
       <c r="M170" t="s">
         <v>1141</v>
       </c>
-      <c r="N170" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>1451</v>
       </c>
@@ -28913,11 +28182,8 @@
       <c r="M171" t="s">
         <v>1041</v>
       </c>
-      <c r="N171" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>1454</v>
       </c>
@@ -28954,11 +28220,8 @@
       <c r="M172" t="s">
         <v>1086</v>
       </c>
-      <c r="N172" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>1457</v>
       </c>
@@ -28995,11 +28258,8 @@
       <c r="M173" t="s">
         <v>1027</v>
       </c>
-      <c r="N173" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>1458</v>
       </c>
@@ -29036,11 +28296,8 @@
       <c r="M174" t="s">
         <v>1124</v>
       </c>
-      <c r="N174" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>1460</v>
       </c>
@@ -29077,11 +28334,8 @@
       <c r="M175" t="s">
         <v>1250</v>
       </c>
-      <c r="N175" t="s">
-        <v>1797</v>
-      </c>
-    </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>1462</v>
       </c>
@@ -29118,11 +28372,8 @@
       <c r="M176" t="s">
         <v>1020</v>
       </c>
-      <c r="N176" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>1465</v>
       </c>
@@ -29159,11 +28410,8 @@
       <c r="M177" t="s">
         <v>1033</v>
       </c>
-      <c r="N177" t="s">
-        <v>1785</v>
-      </c>
-    </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>1469</v>
       </c>
@@ -29200,11 +28448,8 @@
       <c r="M178" t="s">
         <v>1241</v>
       </c>
-      <c r="N178" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>1471</v>
       </c>
@@ -29241,11 +28486,8 @@
       <c r="M179" t="s">
         <v>1141</v>
       </c>
-      <c r="N179" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>1473</v>
       </c>
@@ -29282,11 +28524,8 @@
       <c r="M180" t="s">
         <v>1015</v>
       </c>
-      <c r="N180" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>1475</v>
       </c>
@@ -29323,11 +28562,8 @@
       <c r="M181" t="s">
         <v>1340</v>
       </c>
-      <c r="N181" t="s">
-        <v>1798</v>
-      </c>
-    </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>1477</v>
       </c>
@@ -29364,11 +28600,8 @@
       <c r="M182" t="s">
         <v>1152</v>
       </c>
-      <c r="N182" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>1479</v>
       </c>
@@ -29405,11 +28638,8 @@
       <c r="M183" t="s">
         <v>1399</v>
       </c>
-      <c r="N183" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>1481</v>
       </c>
@@ -29446,11 +28676,8 @@
       <c r="M184" t="s">
         <v>1241</v>
       </c>
-      <c r="N184" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>1483</v>
       </c>
@@ -29487,11 +28714,8 @@
       <c r="M185" t="s">
         <v>1097</v>
       </c>
-      <c r="N185" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>1485</v>
       </c>
@@ -29528,11 +28752,8 @@
       <c r="M186" t="s">
         <v>1067</v>
       </c>
-      <c r="N186" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>1488</v>
       </c>
@@ -29569,11 +28790,8 @@
       <c r="M187" t="s">
         <v>1491</v>
       </c>
-      <c r="N187" t="s">
-        <v>1776</v>
-      </c>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>1492</v>
       </c>
@@ -29610,11 +28828,8 @@
       <c r="M188" t="s">
         <v>1020</v>
       </c>
-      <c r="N188" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>1494</v>
       </c>
@@ -29651,11 +28866,8 @@
       <c r="M189" t="s">
         <v>1409</v>
       </c>
-      <c r="N189" t="s">
-        <v>1801</v>
-      </c>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>1496</v>
       </c>
@@ -29692,11 +28904,8 @@
       <c r="M190" t="s">
         <v>1491</v>
       </c>
-      <c r="N190" t="s">
-        <v>1776</v>
-      </c>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>1499</v>
       </c>
@@ -29733,11 +28942,8 @@
       <c r="M191" t="s">
         <v>1064</v>
       </c>
-      <c r="N191" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>1501</v>
       </c>
@@ -29774,11 +28980,8 @@
       <c r="M192" t="s">
         <v>1420</v>
       </c>
-      <c r="N192" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>1503</v>
       </c>
@@ -29815,11 +29018,8 @@
       <c r="M193" t="s">
         <v>1152</v>
       </c>
-      <c r="N193" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>1505</v>
       </c>
@@ -29856,11 +29056,8 @@
       <c r="M194" t="s">
         <v>1058</v>
       </c>
-      <c r="N194" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>1507</v>
       </c>
@@ -29897,11 +29094,8 @@
       <c r="M195" t="s">
         <v>1064</v>
       </c>
-      <c r="N195" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>1509</v>
       </c>
@@ -29938,11 +29132,8 @@
       <c r="M196" t="s">
         <v>1129</v>
       </c>
-      <c r="N196" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>1511</v>
       </c>
@@ -29979,11 +29170,8 @@
       <c r="M197" t="s">
         <v>1086</v>
       </c>
-      <c r="N197" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>1513</v>
       </c>
@@ -30020,11 +29208,8 @@
       <c r="M198" t="s">
         <v>1113</v>
       </c>
-      <c r="N198" t="s">
-        <v>1792</v>
-      </c>
-    </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>1517</v>
       </c>
@@ -30061,11 +29246,8 @@
       <c r="M199" t="s">
         <v>1078</v>
       </c>
-      <c r="N199" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>1519</v>
       </c>
@@ -30102,11 +29284,8 @@
       <c r="M200" t="s">
         <v>1067</v>
       </c>
-      <c r="N200" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>1521</v>
       </c>
@@ -30143,11 +29322,8 @@
       <c r="M201" t="s">
         <v>1257</v>
       </c>
-      <c r="N201" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>1523</v>
       </c>
@@ -30184,11 +29360,8 @@
       <c r="M202" t="s">
         <v>1067</v>
       </c>
-      <c r="N202" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>1525</v>
       </c>
@@ -30225,11 +29398,8 @@
       <c r="M203" t="s">
         <v>1262</v>
       </c>
-      <c r="N203">
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>1527</v>
       </c>
@@ -30266,11 +29436,8 @@
       <c r="M204" t="s">
         <v>1361</v>
       </c>
-      <c r="N204" t="s">
-        <v>1799</v>
-      </c>
-    </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>1530</v>
       </c>
@@ -30307,11 +29474,8 @@
       <c r="M205" t="s">
         <v>1174</v>
       </c>
-      <c r="N205" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>1532</v>
       </c>
@@ -30348,11 +29512,8 @@
       <c r="M206" t="s">
         <v>1033</v>
       </c>
-      <c r="N206" t="s">
-        <v>1785</v>
-      </c>
-    </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>1535</v>
       </c>
@@ -30389,11 +29550,8 @@
       <c r="M207" t="s">
         <v>1241</v>
       </c>
-      <c r="N207" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>1537</v>
       </c>
@@ -30430,11 +29588,8 @@
       <c r="M208" t="s">
         <v>1086</v>
       </c>
-      <c r="N208" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>1541</v>
       </c>
@@ -30471,11 +29626,8 @@
       <c r="M209" t="s">
         <v>1089</v>
       </c>
-      <c r="N209" t="s">
-        <v>1791</v>
-      </c>
-    </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>1543</v>
       </c>
@@ -30512,11 +29664,8 @@
       <c r="M210" t="s">
         <v>1015</v>
       </c>
-      <c r="N210" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>1545</v>
       </c>
@@ -30553,11 +29702,8 @@
       <c r="M211" t="s">
         <v>1071</v>
       </c>
-      <c r="N211" t="s">
-        <v>1789</v>
-      </c>
-    </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>1547</v>
       </c>
@@ -30594,11 +29740,8 @@
       <c r="M212" t="s">
         <v>1067</v>
       </c>
-      <c r="N212" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>1549</v>
       </c>
@@ -30635,11 +29778,8 @@
       <c r="M213" t="s">
         <v>1409</v>
       </c>
-      <c r="N213" t="s">
-        <v>1801</v>
-      </c>
-    </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>1551</v>
       </c>
@@ -30676,11 +29816,8 @@
       <c r="M214" t="s">
         <v>1328</v>
       </c>
-      <c r="N214" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>1552</v>
       </c>
@@ -30717,11 +29854,8 @@
       <c r="M215" t="s">
         <v>1328</v>
       </c>
-      <c r="N215" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>1553</v>
       </c>
@@ -30758,11 +29892,8 @@
       <c r="M216" t="s">
         <v>1194</v>
       </c>
-      <c r="N216" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>1555</v>
       </c>
@@ -30799,11 +29930,8 @@
       <c r="M217" t="s">
         <v>1097</v>
       </c>
-      <c r="N217" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>1557</v>
       </c>
@@ -30840,11 +29968,8 @@
       <c r="M218" t="s">
         <v>1027</v>
       </c>
-      <c r="N218" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>1559</v>
       </c>
@@ -30881,22 +30006,19 @@
       <c r="M219" t="s">
         <v>1340</v>
       </c>
-      <c r="N219" t="s">
-        <v>1798</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O219" xr:uid="{00000000-0001-0000-0600-000000000000}"/>
+  <autoFilter ref="A1:N219" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G2" sqref="G2:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30912,7 +30034,7 @@
     <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -30940,11 +30062,8 @@
       <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1562</v>
       </c>
@@ -30969,11 +30088,8 @@
       <c r="I2" t="s">
         <v>1141</v>
       </c>
-      <c r="J2" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1565</v>
       </c>
@@ -30998,11 +30114,8 @@
       <c r="I3" t="s">
         <v>1052</v>
       </c>
-      <c r="J3" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1567</v>
       </c>
@@ -31027,11 +30140,8 @@
       <c r="I4" t="s">
         <v>1285</v>
       </c>
-      <c r="J4" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1569</v>
       </c>
@@ -31056,11 +30166,8 @@
       <c r="I5" t="s">
         <v>1058</v>
       </c>
-      <c r="J5" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1571</v>
       </c>
@@ -31085,11 +30192,8 @@
       <c r="I6" t="s">
         <v>1155</v>
       </c>
-      <c r="J6" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1573</v>
       </c>
@@ -31114,11 +30218,8 @@
       <c r="I7" t="s">
         <v>1253</v>
       </c>
-      <c r="J7" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1575</v>
       </c>
@@ -31143,11 +30244,8 @@
       <c r="I8" t="s">
         <v>1097</v>
       </c>
-      <c r="J8" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1577</v>
       </c>
@@ -31172,11 +30270,8 @@
       <c r="I9" t="s">
         <v>1027</v>
       </c>
-      <c r="J9" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1579</v>
       </c>
@@ -31201,11 +30296,8 @@
       <c r="I10" t="s">
         <v>1041</v>
       </c>
-      <c r="J10" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1581</v>
       </c>
@@ -31230,11 +30322,8 @@
       <c r="I11" t="s">
         <v>1583</v>
       </c>
-      <c r="J11" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1584</v>
       </c>
@@ -31259,11 +30348,8 @@
       <c r="I12" t="s">
         <v>1081</v>
       </c>
-      <c r="J12" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1586</v>
       </c>
@@ -31288,11 +30374,8 @@
       <c r="I13" t="s">
         <v>1024</v>
       </c>
-      <c r="J13" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1588</v>
       </c>
@@ -31317,11 +30400,8 @@
       <c r="I14" t="s">
         <v>1155</v>
       </c>
-      <c r="J14" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1591</v>
       </c>
@@ -31346,11 +30426,8 @@
       <c r="I15" t="s">
         <v>1027</v>
       </c>
-      <c r="J15" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1593</v>
       </c>
@@ -31375,11 +30452,8 @@
       <c r="I16" t="s">
         <v>1491</v>
       </c>
-      <c r="J16" t="s">
-        <v>1776</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>1595</v>
       </c>
@@ -31404,11 +30478,8 @@
       <c r="I17" t="s">
         <v>1262</v>
       </c>
-      <c r="J17" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1597</v>
       </c>
@@ -31433,11 +30504,8 @@
       <c r="I18" t="s">
         <v>1058</v>
       </c>
-      <c r="J18" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1599</v>
       </c>
@@ -31462,11 +30530,8 @@
       <c r="I19" t="s">
         <v>1328</v>
       </c>
-      <c r="J19" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1601</v>
       </c>
@@ -31491,11 +30556,8 @@
       <c r="I20" t="s">
         <v>1027</v>
       </c>
-      <c r="J20" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1603</v>
       </c>
@@ -31520,11 +30582,8 @@
       <c r="I21" t="s">
         <v>1041</v>
       </c>
-      <c r="J21" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1605</v>
       </c>
@@ -31549,11 +30608,8 @@
       <c r="I22" t="s">
         <v>1075</v>
       </c>
-      <c r="J22" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1607</v>
       </c>
@@ -31578,11 +30634,8 @@
       <c r="I23" t="s">
         <v>1097</v>
       </c>
-      <c r="J23" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1609</v>
       </c>
@@ -31607,11 +30660,8 @@
       <c r="I24" t="s">
         <v>1611</v>
       </c>
-      <c r="J24" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1612</v>
       </c>
@@ -31636,11 +30686,8 @@
       <c r="I25" t="s">
         <v>1174</v>
       </c>
-      <c r="J25" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1614</v>
       </c>
@@ -31665,11 +30712,8 @@
       <c r="I26" t="s">
         <v>1058</v>
       </c>
-      <c r="J26" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1616</v>
       </c>
@@ -31694,11 +30738,8 @@
       <c r="I27" t="s">
         <v>1081</v>
       </c>
-      <c r="J27" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1618</v>
       </c>
@@ -31723,11 +30764,8 @@
       <c r="I28" t="s">
         <v>1049</v>
       </c>
-      <c r="J28" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1620</v>
       </c>
@@ -31752,11 +30790,8 @@
       <c r="I29" t="s">
         <v>1328</v>
       </c>
-      <c r="J29" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1621</v>
       </c>
@@ -31781,11 +30816,8 @@
       <c r="I30" t="s">
         <v>1041</v>
       </c>
-      <c r="J30" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1623</v>
       </c>
@@ -31810,11 +30842,8 @@
       <c r="I31" t="s">
         <v>1141</v>
       </c>
-      <c r="J31" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1625</v>
       </c>
@@ -31839,11 +30868,8 @@
       <c r="I32" t="s">
         <v>1081</v>
       </c>
-      <c r="J32" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1626</v>
       </c>
@@ -31868,11 +30894,8 @@
       <c r="I33" t="s">
         <v>1094</v>
       </c>
-      <c r="J33" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>1628</v>
       </c>
@@ -31897,11 +30920,8 @@
       <c r="I34" t="s">
         <v>1630</v>
       </c>
-      <c r="J34" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>1631</v>
       </c>
@@ -31926,11 +30946,8 @@
       <c r="I35" t="s">
         <v>1094</v>
       </c>
-      <c r="J35" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1633</v>
       </c>
@@ -31955,11 +30972,8 @@
       <c r="I36" t="s">
         <v>1630</v>
       </c>
-      <c r="J36" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>1635</v>
       </c>
@@ -31984,11 +30998,8 @@
       <c r="I37" t="s">
         <v>1637</v>
       </c>
-      <c r="J37" t="s">
-        <v>1780</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>1638</v>
       </c>
@@ -32013,11 +31024,8 @@
       <c r="I38" t="s">
         <v>1216</v>
       </c>
-      <c r="J38" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>1640</v>
       </c>
@@ -32042,11 +31050,8 @@
       <c r="I39" t="s">
         <v>1078</v>
       </c>
-      <c r="J39" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>1642</v>
       </c>
@@ -32071,11 +31076,8 @@
       <c r="I40" t="s">
         <v>1119</v>
       </c>
-      <c r="J40" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>1644</v>
       </c>
@@ -32100,11 +31102,8 @@
       <c r="I41" t="s">
         <v>1637</v>
       </c>
-      <c r="J41" t="s">
-        <v>1780</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>1646</v>
       </c>
@@ -32129,11 +31128,8 @@
       <c r="I42" t="s">
         <v>1078</v>
       </c>
-      <c r="J42" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>1648</v>
       </c>
@@ -32158,11 +31154,8 @@
       <c r="I43" t="s">
         <v>1097</v>
       </c>
-      <c r="J43" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>1650</v>
       </c>
@@ -32187,11 +31180,8 @@
       <c r="I44" t="s">
         <v>1027</v>
       </c>
-      <c r="J44" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1651</v>
       </c>
@@ -32216,12 +31206,9 @@
       <c r="I45" t="s">
         <v>1630</v>
       </c>
-      <c r="J45" t="s">
-        <v>1775</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J45" xr:uid="{00000000-0001-0000-0700-000000000000}"/>
+  <autoFilter ref="A1:I45" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -32229,10 +31216,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32244,7 +31231,7 @@
     <col min="14" max="14" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -32278,11 +31265,8 @@
       <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1655</v>
       </c>
@@ -32316,11 +31300,8 @@
       <c r="K2" t="s">
         <v>1124</v>
       </c>
-      <c r="L2" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1658</v>
       </c>
@@ -32354,11 +31335,8 @@
       <c r="K3" t="s">
         <v>1152</v>
       </c>
-      <c r="L3" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1660</v>
       </c>
@@ -32392,11 +31370,8 @@
       <c r="K4" t="s">
         <v>1124</v>
       </c>
-      <c r="L4" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1662</v>
       </c>
@@ -32430,11 +31405,8 @@
       <c r="K5" t="s">
         <v>1124</v>
       </c>
-      <c r="L5" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1664</v>
       </c>
@@ -32468,11 +31440,8 @@
       <c r="K6" t="s">
         <v>1205</v>
       </c>
-      <c r="L6" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1667</v>
       </c>
@@ -32506,11 +31475,8 @@
       <c r="K7" t="s">
         <v>1124</v>
       </c>
-      <c r="L7" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1669</v>
       </c>
@@ -32544,11 +31510,8 @@
       <c r="K8" t="s">
         <v>1124</v>
       </c>
-      <c r="L8" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1671</v>
       </c>
@@ -32582,11 +31545,8 @@
       <c r="K9" t="s">
         <v>1124</v>
       </c>
-      <c r="L9" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1673</v>
       </c>
@@ -32620,11 +31580,8 @@
       <c r="K10" t="s">
         <v>1205</v>
       </c>
-      <c r="L10" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1675</v>
       </c>
@@ -32658,11 +31615,8 @@
       <c r="K11" t="s">
         <v>1124</v>
       </c>
-      <c r="L11" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1677</v>
       </c>
@@ -32696,12 +31650,9 @@
       <c r="K12" t="s">
         <v>1124</v>
       </c>
-      <c r="L12" t="s">
-        <v>1765</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L12" xr:uid="{00000000-0001-0000-0800-000000000000}"/>
+  <autoFilter ref="A1:K14" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ensure product searches work reliably by fixing category-specific filters
Modify conditional rendering for max_door_width in index.html to ensure accurate filtering for Bathtubs and Shower Bases.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/e6886a28-8571-453f-8960-8340201fe34a.jpg
</commit_message>
<xml_diff>
--- a/data/Product Data.xlsx
+++ b/data/Product Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/PythonScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64A92024-551F-4F9D-8C01-7B670142FAF5}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="11_BCFEBD4F73F15EB6C55EF89F1835901893D73E67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{403A3A97-9E76-417F-8C49-724C610E699D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2565" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shower Bases" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Enclosures!$A$1:$L$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Return Panels'!$A$1:$F$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Screens!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Shower Bases'!$A$1:$O$221</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Shower Doors'!$A$1:$O$158</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Showers!$A$1:$I$151</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Tub Doors'!$A$1:$L$36</definedName>
@@ -5056,9 +5057,6 @@
     <t>https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/websites-product-info-and-content/maax/products/walls/103414/images/maax-103414-300-502.jpg</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/websites-product-info-and-content/maax/products/doors/136335/images/maax-136335-975-340.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/websites-product-info-and-content/maax/products/doors/136679/images/maax-136679-900-084.jpg</t>
   </si>
   <si>
@@ -5581,9 +5579,6 @@
     <t>https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/websites-product-info-and-content/maax/products/doors/139582/images/maax-139582-900-305.jpg</t>
   </si>
   <si>
-    <t>https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1667924901/abg-graphics/original-images/maax/multi-brand/doors/duel/jpeg/mixed-finish/duel-ts-exhibit-ch-mb.jpg</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/websites-product-info-and-content/maax/products/bathtubs/105821/images/maax-105821-001.jpg</t>
   </si>
   <si>
@@ -6152,6 +6147,12 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/american-bath-group/image/upload/v1695151236/abg-graphics/original-images/maax/showroom/Collection/doors/capella/capella-32rp-bn-crop.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/american-bath-group/image/upload/websites-product-info-and-content/maax/products/doors/136335/images/maax-136335-975-340.jpg</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/american-bath-group/image/upload/v1667924901/abg-graphics/original-images/maax/multi-brand/doors/duel/jpeg/mixed-finish/duel-ts-exhibit-ch-mb.jpg</t>
   </si>
 </sst>
 </file>
@@ -6264,6 +6265,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6531,8 +6536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="A222" sqref="A222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14951,6 +14956,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O221" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -15002,7 +15008,7 @@
         <v>1425</v>
       </c>
       <c r="C2" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1078</v>
@@ -15022,7 +15028,7 @@
         <v>1426</v>
       </c>
       <c r="C3" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1154</v>
@@ -15042,7 +15048,7 @@
         <v>1427</v>
       </c>
       <c r="C4" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1083</v>
@@ -15062,7 +15068,7 @@
         <v>1428</v>
       </c>
       <c r="C5" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1083</v>
@@ -15082,7 +15088,7 @@
         <v>1429</v>
       </c>
       <c r="C6" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1078</v>
@@ -15102,7 +15108,7 @@
         <v>1431</v>
       </c>
       <c r="C7" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1091</v>
@@ -15122,7 +15128,7 @@
         <v>1432</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>2030</v>
+        <v>2028</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1078</v>
@@ -15142,7 +15148,7 @@
         <v>1433</v>
       </c>
       <c r="C9" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>1078</v>
@@ -15162,7 +15168,7 @@
         <v>1434</v>
       </c>
       <c r="C10" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1078</v>
@@ -15182,7 +15188,7 @@
         <v>1435</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>2031</v>
+        <v>2029</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1083</v>
@@ -15202,7 +15208,7 @@
         <v>1436</v>
       </c>
       <c r="C12" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1078</v>
@@ -15222,7 +15228,7 @@
         <v>1437</v>
       </c>
       <c r="C13" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1154</v>
@@ -15242,7 +15248,7 @@
         <v>1438</v>
       </c>
       <c r="C14" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1083</v>
@@ -15262,7 +15268,7 @@
         <v>1439</v>
       </c>
       <c r="C15" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1078</v>
@@ -15282,7 +15288,7 @@
         <v>1440</v>
       </c>
       <c r="C16" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1083</v>
@@ -15302,7 +15308,7 @@
         <v>1441</v>
       </c>
       <c r="C17" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>797</v>
@@ -15322,7 +15328,7 @@
         <v>1442</v>
       </c>
       <c r="C18" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1083</v>
@@ -15342,7 +15348,7 @@
         <v>1443</v>
       </c>
       <c r="C19" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1154</v>
@@ -15362,7 +15368,7 @@
         <v>1444</v>
       </c>
       <c r="C20" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>1083</v>
@@ -15382,7 +15388,7 @@
         <v>1445</v>
       </c>
       <c r="C21" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>1083</v>
@@ -15402,7 +15408,7 @@
         <v>1446</v>
       </c>
       <c r="C22" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1083</v>
@@ -15422,7 +15428,7 @@
         <v>1447</v>
       </c>
       <c r="C23" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1083</v>
@@ -15442,7 +15448,7 @@
         <v>1448</v>
       </c>
       <c r="C24" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1083</v>
@@ -15462,7 +15468,7 @@
         <v>1449</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>2032</v>
+        <v>2030</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>1078</v>
@@ -15482,7 +15488,7 @@
         <v>1450</v>
       </c>
       <c r="C26" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>1078</v>
@@ -15502,7 +15508,7 @@
         <v>1451</v>
       </c>
       <c r="C27" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1078</v>
@@ -15522,7 +15528,7 @@
         <v>1452</v>
       </c>
       <c r="C28" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>1078</v>
@@ -15542,7 +15548,7 @@
         <v>1453</v>
       </c>
       <c r="C29" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>1154</v>
@@ -15569,8 +15575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N146"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15643,7 +15649,7 @@
         <v>291</v>
       </c>
       <c r="C2" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="E2">
         <v>58.375</v>
@@ -15678,7 +15684,7 @@
         <v>294</v>
       </c>
       <c r="C3" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="E3">
         <v>58.25</v>
@@ -15713,7 +15719,7 @@
         <v>297</v>
       </c>
       <c r="C4" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="E4">
         <v>58.375</v>
@@ -15748,7 +15754,7 @@
         <v>299</v>
       </c>
       <c r="C5" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
       <c r="E5">
         <v>58.375</v>
@@ -15783,7 +15789,7 @@
         <v>301</v>
       </c>
       <c r="C6" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="E6">
         <v>58.375</v>
@@ -15818,7 +15824,7 @@
         <v>303</v>
       </c>
       <c r="C7" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="E7">
         <v>58.25</v>
@@ -15853,7 +15859,7 @@
         <v>304</v>
       </c>
       <c r="C8" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="E8">
         <v>58.375</v>
@@ -15888,7 +15894,7 @@
         <v>305</v>
       </c>
       <c r="C9" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
       <c r="E9">
         <v>58.125</v>
@@ -15923,7 +15929,7 @@
         <v>307</v>
       </c>
       <c r="C10" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="E10">
         <v>58.375</v>
@@ -15958,7 +15964,7 @@
         <v>308</v>
       </c>
       <c r="C11" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
       <c r="E11">
         <v>58.25</v>
@@ -15993,7 +15999,7 @@
         <v>310</v>
       </c>
       <c r="C12" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
       <c r="E12">
         <v>58.375</v>
@@ -16028,7 +16034,7 @@
         <v>311</v>
       </c>
       <c r="C13" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
       <c r="E13">
         <v>64.375</v>
@@ -16063,7 +16069,7 @@
         <v>313</v>
       </c>
       <c r="C14" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
       <c r="E14">
         <v>58.375</v>
@@ -16098,7 +16104,7 @@
         <v>315</v>
       </c>
       <c r="C15" t="s">
-        <v>1856</v>
+        <v>1854</v>
       </c>
       <c r="E15">
         <v>64.75</v>
@@ -16133,7 +16139,7 @@
         <v>318</v>
       </c>
       <c r="C16" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
       <c r="E16">
         <v>64.375</v>
@@ -16168,7 +16174,7 @@
         <v>319</v>
       </c>
       <c r="C17" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="E17">
         <v>71.375</v>
@@ -16203,7 +16209,7 @@
         <v>320</v>
       </c>
       <c r="C18" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
       <c r="E18">
         <v>59.375</v>
@@ -16238,7 +16244,7 @@
         <v>321</v>
       </c>
       <c r="C19" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
       <c r="E19">
         <v>58.25</v>
@@ -16273,7 +16279,7 @@
         <v>323</v>
       </c>
       <c r="C20" t="s">
-        <v>1861</v>
+        <v>1859</v>
       </c>
       <c r="E20">
         <v>58.25</v>
@@ -16308,7 +16314,7 @@
         <v>324</v>
       </c>
       <c r="C21" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
       <c r="E21">
         <v>58.25</v>
@@ -16343,7 +16349,7 @@
         <v>327</v>
       </c>
       <c r="C22" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="E22">
         <v>70.125</v>
@@ -16378,7 +16384,7 @@
         <v>328</v>
       </c>
       <c r="C23" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="E23">
         <v>58.25</v>
@@ -16413,7 +16419,7 @@
         <v>330</v>
       </c>
       <c r="C24" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
       <c r="E24">
         <v>64.25</v>
@@ -16448,7 +16454,7 @@
         <v>331</v>
       </c>
       <c r="C25" t="s">
-        <v>1866</v>
+        <v>1864</v>
       </c>
       <c r="E25">
         <v>58.375</v>
@@ -16483,7 +16489,7 @@
         <v>333</v>
       </c>
       <c r="C26" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="E26">
         <v>70</v>
@@ -16518,7 +16524,7 @@
         <v>335</v>
       </c>
       <c r="C27" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="E27">
         <v>58.25</v>
@@ -16553,7 +16559,7 @@
         <v>336</v>
       </c>
       <c r="C28" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="E28">
         <v>70.125</v>
@@ -16588,7 +16594,7 @@
         <v>337</v>
       </c>
       <c r="C29" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
       <c r="E29">
         <v>70.375</v>
@@ -16623,7 +16629,7 @@
         <v>339</v>
       </c>
       <c r="C30" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="E30">
         <v>58.375</v>
@@ -16658,7 +16664,7 @@
         <v>341</v>
       </c>
       <c r="C31" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="E31">
         <v>65.75</v>
@@ -16693,7 +16699,7 @@
         <v>342</v>
       </c>
       <c r="C32" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="E32">
         <v>58.375</v>
@@ -16728,7 +16734,7 @@
         <v>343</v>
       </c>
       <c r="C33" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="E33">
         <v>70.375</v>
@@ -16763,7 +16769,7 @@
         <v>344</v>
       </c>
       <c r="C34" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="E34">
         <v>58.25</v>
@@ -16798,7 +16804,7 @@
         <v>346</v>
       </c>
       <c r="C35" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="E35">
         <v>70.375</v>
@@ -16833,7 +16839,7 @@
         <v>330</v>
       </c>
       <c r="C36" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="E36">
         <v>64.25</v>
@@ -16868,7 +16874,7 @@
         <v>347</v>
       </c>
       <c r="C37" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="E37">
         <v>58.25</v>
@@ -16903,7 +16909,7 @@
         <v>348</v>
       </c>
       <c r="C38" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="E38">
         <v>70.375</v>
@@ -16938,7 +16944,7 @@
         <v>333</v>
       </c>
       <c r="C39" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="E39">
         <v>70</v>
@@ -16973,7 +16979,7 @@
         <v>349</v>
       </c>
       <c r="C40" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="E40">
         <v>58.25</v>
@@ -17008,7 +17014,7 @@
         <v>350</v>
       </c>
       <c r="C41" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
       <c r="E41">
         <v>70.375</v>
@@ -17043,7 +17049,7 @@
         <v>351</v>
       </c>
       <c r="C42" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
       <c r="E42">
         <v>58.25</v>
@@ -17078,7 +17084,7 @@
         <v>352</v>
       </c>
       <c r="C43" t="s">
-        <v>1884</v>
+        <v>1882</v>
       </c>
       <c r="E43">
         <v>65.375</v>
@@ -17113,7 +17119,7 @@
         <v>353</v>
       </c>
       <c r="C44" t="s">
-        <v>1885</v>
+        <v>1883</v>
       </c>
       <c r="E44">
         <v>58.25</v>
@@ -17148,7 +17154,7 @@
         <v>354</v>
       </c>
       <c r="C45" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
       <c r="E45">
         <v>70.375</v>
@@ -17183,7 +17189,7 @@
         <v>355</v>
       </c>
       <c r="C46" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="E46">
         <v>58.25</v>
@@ -17218,7 +17224,7 @@
         <v>356</v>
       </c>
       <c r="C47" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
       <c r="E47">
         <v>58.375</v>
@@ -17253,7 +17259,7 @@
         <v>358</v>
       </c>
       <c r="C48" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="E48">
         <v>58.25</v>
@@ -17288,7 +17294,7 @@
         <v>359</v>
       </c>
       <c r="C49" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
       <c r="E49">
         <v>70.375</v>
@@ -17323,7 +17329,7 @@
         <v>360</v>
       </c>
       <c r="C50" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="E50">
         <v>58.125</v>
@@ -17358,7 +17364,7 @@
         <v>294</v>
       </c>
       <c r="C51" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
       <c r="E51">
         <v>58.375</v>
@@ -17393,7 +17399,7 @@
         <v>362</v>
       </c>
       <c r="C52" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="E52">
         <v>70.375</v>
@@ -17428,7 +17434,7 @@
         <v>363</v>
       </c>
       <c r="C53" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="E53">
         <v>70.375</v>
@@ -17463,7 +17469,7 @@
         <v>364</v>
       </c>
       <c r="C54" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="E54">
         <v>58.375</v>
@@ -17498,7 +17504,7 @@
         <v>365</v>
       </c>
       <c r="C55" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="E55">
         <v>58.375</v>
@@ -17533,7 +17539,7 @@
         <v>366</v>
       </c>
       <c r="C56" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
       <c r="E56">
         <v>58.375</v>
@@ -17568,7 +17574,7 @@
         <v>367</v>
       </c>
       <c r="C57" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
       <c r="E57">
         <v>64.375</v>
@@ -17603,7 +17609,7 @@
         <v>368</v>
       </c>
       <c r="C58" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="E58">
         <v>70.375</v>
@@ -17638,7 +17644,7 @@
         <v>369</v>
       </c>
       <c r="C59" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
       <c r="E59">
         <v>58.375</v>
@@ -17673,7 +17679,7 @@
         <v>370</v>
       </c>
       <c r="C60" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="E60">
         <v>58.25</v>
@@ -17708,7 +17714,7 @@
         <v>372</v>
       </c>
       <c r="C61" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="E61">
         <v>70.375</v>
@@ -17743,7 +17749,7 @@
         <v>373</v>
       </c>
       <c r="C62" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="E62">
         <v>58.375</v>
@@ -17778,7 +17784,7 @@
         <v>305</v>
       </c>
       <c r="C63" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
       <c r="E63">
         <v>58.125</v>
@@ -17813,7 +17819,7 @@
         <v>374</v>
       </c>
       <c r="C64" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="E64">
         <v>64.375</v>
@@ -17848,7 +17854,7 @@
         <v>375</v>
       </c>
       <c r="C65" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="E65">
         <v>58.375</v>
@@ -17883,7 +17889,7 @@
         <v>333</v>
       </c>
       <c r="C66" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="E66">
         <v>70.5</v>
@@ -17918,7 +17924,7 @@
         <v>376</v>
       </c>
       <c r="C67" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="E67">
         <v>70.5</v>
@@ -17953,7 +17959,7 @@
         <v>379</v>
       </c>
       <c r="C68" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
       <c r="E68">
         <v>58.375</v>
@@ -17988,7 +17994,7 @@
         <v>380</v>
       </c>
       <c r="C69" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="E69">
         <v>58.25</v>
@@ -18023,7 +18029,7 @@
         <v>381</v>
       </c>
       <c r="C70" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="E70">
         <v>58.25</v>
@@ -18058,7 +18064,7 @@
         <v>382</v>
       </c>
       <c r="C71" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="E71">
         <v>64.25</v>
@@ -18093,7 +18099,7 @@
         <v>383</v>
       </c>
       <c r="C72" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="E72">
         <v>58.25</v>
@@ -18128,7 +18134,7 @@
         <v>384</v>
       </c>
       <c r="C73" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="E73">
         <v>64.25</v>
@@ -18163,7 +18169,7 @@
         <v>385</v>
       </c>
       <c r="C74" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="E74">
         <v>58.25</v>
@@ -18198,7 +18204,7 @@
         <v>386</v>
       </c>
       <c r="C75" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="E75">
         <v>70</v>
@@ -18233,7 +18239,7 @@
         <v>388</v>
       </c>
       <c r="C76" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="E76">
         <v>58.5</v>
@@ -18268,7 +18274,7 @@
         <v>386</v>
       </c>
       <c r="C77" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="E77">
         <v>70</v>
@@ -18303,7 +18309,7 @@
         <v>389</v>
       </c>
       <c r="C78" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="E78">
         <v>59.75</v>
@@ -18338,7 +18344,7 @@
         <v>390</v>
       </c>
       <c r="C79" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="E79">
         <v>58.375</v>
@@ -18373,7 +18379,7 @@
         <v>391</v>
       </c>
       <c r="C80" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
       <c r="E80">
         <v>58.25</v>
@@ -18408,7 +18414,7 @@
         <v>330</v>
       </c>
       <c r="C81" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="E81">
         <v>64.25</v>
@@ -18443,7 +18449,7 @@
         <v>393</v>
       </c>
       <c r="C82" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="E82">
         <v>58.375</v>
@@ -18478,7 +18484,7 @@
         <v>382</v>
       </c>
       <c r="C83" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="E83">
         <v>64.25</v>
@@ -18513,7 +18519,7 @@
         <v>394</v>
       </c>
       <c r="C84" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="E84">
         <v>58.375</v>
@@ -18548,7 +18554,7 @@
         <v>395</v>
       </c>
       <c r="C85" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="E85">
         <v>70.375</v>
@@ -18583,7 +18589,7 @@
         <v>360</v>
       </c>
       <c r="C86" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
       <c r="E86">
         <v>58.125</v>
@@ -18618,7 +18624,7 @@
         <v>396</v>
       </c>
       <c r="C87" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="E87">
         <v>58.375</v>
@@ -18653,7 +18659,7 @@
         <v>305</v>
       </c>
       <c r="C88" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="E88">
         <v>58.125</v>
@@ -18688,7 +18694,7 @@
         <v>397</v>
       </c>
       <c r="C89" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="E89">
         <v>58.25</v>
@@ -18723,7 +18729,7 @@
         <v>398</v>
       </c>
       <c r="C90" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="E90">
         <v>70.375</v>
@@ -18758,7 +18764,7 @@
         <v>399</v>
       </c>
       <c r="C91" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
       <c r="E91">
         <v>64.375</v>
@@ -18793,7 +18799,7 @@
         <v>304</v>
       </c>
       <c r="C92" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="E92">
         <v>58.25</v>
@@ -18828,7 +18834,7 @@
         <v>386</v>
       </c>
       <c r="C93" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
       <c r="E93">
         <v>70</v>
@@ -18863,7 +18869,7 @@
         <v>401</v>
       </c>
       <c r="C94" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="E94">
         <v>58.375</v>
@@ -18898,7 +18904,7 @@
         <v>402</v>
       </c>
       <c r="C95" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="E95">
         <v>58.25</v>
@@ -18933,7 +18939,7 @@
         <v>403</v>
       </c>
       <c r="C96" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="E96">
         <v>70.375</v>
@@ -18968,7 +18974,7 @@
         <v>404</v>
       </c>
       <c r="C97" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
       <c r="E97">
         <v>58.25</v>
@@ -19003,7 +19009,7 @@
         <v>405</v>
       </c>
       <c r="C98" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E98">
         <v>64.375</v>
@@ -19038,7 +19044,7 @@
         <v>406</v>
       </c>
       <c r="C99" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="E99">
         <v>70.5</v>
@@ -19073,7 +19079,7 @@
         <v>407</v>
       </c>
       <c r="C100" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
       <c r="E100">
         <v>58.375</v>
@@ -19108,7 +19114,7 @@
         <v>301</v>
       </c>
       <c r="C101" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="E101">
         <v>58.25</v>
@@ -19143,7 +19149,7 @@
         <v>409</v>
       </c>
       <c r="C102" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="E102">
         <v>70.375</v>
@@ -19178,7 +19184,7 @@
         <v>360</v>
       </c>
       <c r="C103" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="E103">
         <v>58.125</v>
@@ -19213,7 +19219,7 @@
         <v>410</v>
       </c>
       <c r="C104" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="E104">
         <v>58.375</v>
@@ -19248,7 +19254,7 @@
         <v>365</v>
       </c>
       <c r="C105" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="E105">
         <v>58.25</v>
@@ -19283,7 +19289,7 @@
         <v>411</v>
       </c>
       <c r="C106" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="E106">
         <v>58.25</v>
@@ -19318,7 +19324,7 @@
         <v>412</v>
       </c>
       <c r="C107" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="E107">
         <v>58.25</v>
@@ -19353,7 +19359,7 @@
         <v>413</v>
       </c>
       <c r="C108" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="E108">
         <v>58.375</v>
@@ -19388,7 +19394,7 @@
         <v>414</v>
       </c>
       <c r="C109" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="E109">
         <v>58.25</v>
@@ -19423,7 +19429,7 @@
         <v>415</v>
       </c>
       <c r="C110" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="E110">
         <v>58.25</v>
@@ -19458,7 +19464,7 @@
         <v>410</v>
       </c>
       <c r="C111" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="E111">
         <v>58.25</v>
@@ -19493,7 +19499,7 @@
         <v>416</v>
       </c>
       <c r="C112" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="E112">
         <v>57</v>
@@ -19528,7 +19534,7 @@
         <v>418</v>
       </c>
       <c r="C113" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="E113">
         <v>58.25</v>
@@ -19563,7 +19569,7 @@
         <v>420</v>
       </c>
       <c r="C114" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="E114">
         <v>58.375</v>
@@ -19598,7 +19604,7 @@
         <v>421</v>
       </c>
       <c r="C115" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="E115">
         <v>65.375</v>
@@ -19633,7 +19639,7 @@
         <v>364</v>
       </c>
       <c r="C116" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="E116">
         <v>58.25</v>
@@ -19668,7 +19674,7 @@
         <v>422</v>
       </c>
       <c r="C117" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="E117">
         <v>64.25</v>
@@ -19703,7 +19709,7 @@
         <v>423</v>
       </c>
       <c r="C118" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="E118">
         <v>64.375</v>
@@ -19738,7 +19744,7 @@
         <v>424</v>
       </c>
       <c r="C119" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="E119">
         <v>57</v>
@@ -19773,7 +19779,7 @@
         <v>425</v>
       </c>
       <c r="C120" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="E120">
         <v>70.375</v>
@@ -19808,7 +19814,7 @@
         <v>426</v>
       </c>
       <c r="C121" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="E121">
         <v>58.25</v>
@@ -19843,7 +19849,7 @@
         <v>427</v>
       </c>
       <c r="C122" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="E122">
         <v>70</v>
@@ -19878,7 +19884,7 @@
         <v>428</v>
       </c>
       <c r="C123" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="E123">
         <v>64.75</v>
@@ -19913,7 +19919,7 @@
         <v>429</v>
       </c>
       <c r="C124" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="E124">
         <v>58.25</v>
@@ -19948,7 +19954,7 @@
         <v>430</v>
       </c>
       <c r="C125" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
       <c r="E125">
         <v>58.375</v>
@@ -19983,7 +19989,7 @@
         <v>431</v>
       </c>
       <c r="C126" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="E126">
         <v>64.375</v>
@@ -20018,7 +20024,7 @@
         <v>432</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>1986</v>
+        <v>1984</v>
       </c>
       <c r="E127">
         <v>56.875</v>
@@ -20050,7 +20056,7 @@
         <v>394</v>
       </c>
       <c r="C128" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
       <c r="E128">
         <v>58.25</v>
@@ -20085,7 +20091,7 @@
         <v>434</v>
       </c>
       <c r="C129" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="E129">
         <v>58.375</v>
@@ -20120,7 +20126,7 @@
         <v>373</v>
       </c>
       <c r="C130" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="E130">
         <v>58.25</v>
@@ -20155,7 +20161,7 @@
         <v>436</v>
       </c>
       <c r="C131" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="E131">
         <v>58.375</v>
@@ -20190,7 +20196,7 @@
         <v>437</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="E132">
         <v>58.25</v>
@@ -20225,7 +20231,7 @@
         <v>439</v>
       </c>
       <c r="C133" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
       <c r="E133">
         <v>59.25</v>
@@ -20260,7 +20266,7 @@
         <v>440</v>
       </c>
       <c r="C134" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
       <c r="E134">
         <v>58.25</v>
@@ -20295,7 +20301,7 @@
         <v>441</v>
       </c>
       <c r="C135" t="s">
-        <v>1974</v>
+        <v>1972</v>
       </c>
       <c r="E135">
         <v>64.375</v>
@@ -20330,7 +20336,7 @@
         <v>442</v>
       </c>
       <c r="C136" t="s">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="E136">
         <v>70.375</v>
@@ -20365,7 +20371,7 @@
         <v>443</v>
       </c>
       <c r="C137" t="s">
-        <v>1976</v>
+        <v>1974</v>
       </c>
       <c r="E137">
         <v>58.375</v>
@@ -20400,7 +20406,7 @@
         <v>444</v>
       </c>
       <c r="C138" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="E138">
         <v>59.75</v>
@@ -20435,7 +20441,7 @@
         <v>382</v>
       </c>
       <c r="C139" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="E139">
         <v>64.25</v>
@@ -20470,7 +20476,7 @@
         <v>445</v>
       </c>
       <c r="C140" t="s">
-        <v>1979</v>
+        <v>1977</v>
       </c>
       <c r="E140">
         <v>64.375</v>
@@ -20505,7 +20511,7 @@
         <v>446</v>
       </c>
       <c r="C141" t="s">
-        <v>1980</v>
+        <v>1978</v>
       </c>
       <c r="E141">
         <v>58.25</v>
@@ -20540,7 +20546,7 @@
         <v>447</v>
       </c>
       <c r="C142" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="E142">
         <v>70.75</v>
@@ -20575,7 +20581,7 @@
         <v>448</v>
       </c>
       <c r="C143" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="E143">
         <v>64.375</v>
@@ -20610,7 +20616,7 @@
         <v>449</v>
       </c>
       <c r="C144" t="s">
-        <v>1983</v>
+        <v>1981</v>
       </c>
       <c r="E144">
         <v>58.25</v>
@@ -20645,7 +20651,7 @@
         <v>450</v>
       </c>
       <c r="C145" t="s">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="E145">
         <v>70.375</v>
@@ -20680,7 +20686,7 @@
         <v>451</v>
       </c>
       <c r="C146" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="E146">
         <v>58.25</v>
@@ -25599,23 +25605,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet5" filterMode="1"/>
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="179.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
     <col min="9" max="9" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
@@ -25661,7 +25667,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>107455</v>
       </c>
@@ -25699,7 +25705,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>107464</v>
       </c>
@@ -25737,7 +25743,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>107458</v>
       </c>
@@ -25775,7 +25781,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>107456</v>
       </c>
@@ -25851,7 +25857,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>107457</v>
       </c>
@@ -25889,7 +25895,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>107466</v>
       </c>
@@ -25927,7 +25933,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>141427</v>
       </c>
@@ -25965,7 +25971,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>141425</v>
       </c>
@@ -26003,7 +26009,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>107460</v>
       </c>
@@ -26041,7 +26047,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>107479</v>
       </c>
@@ -26079,7 +26085,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>107352</v>
       </c>
@@ -26117,7 +26123,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>107461</v>
       </c>
@@ -26155,7 +26161,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>107462</v>
       </c>
@@ -26193,7 +26199,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>107228</v>
       </c>
@@ -26231,7 +26237,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>107465</v>
       </c>
@@ -26239,7 +26245,7 @@
         <v>1084</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -26307,7 +26313,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>107459</v>
       </c>
@@ -26345,7 +26351,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>103408</v>
       </c>
@@ -26383,7 +26389,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>103418</v>
       </c>
@@ -26421,7 +26427,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>107227</v>
       </c>
@@ -26497,7 +26503,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>107224</v>
       </c>
@@ -26535,7 +26541,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>103424</v>
       </c>
@@ -26611,7 +26617,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>107144</v>
       </c>
@@ -26649,7 +26655,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>107140</v>
       </c>
@@ -26687,7 +26693,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>103388</v>
       </c>
@@ -26725,7 +26731,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>107463</v>
       </c>
@@ -26763,7 +26769,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>107223</v>
       </c>
@@ -26801,7 +26807,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>106542</v>
       </c>
@@ -26839,7 +26845,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>103378</v>
       </c>
@@ -26877,7 +26883,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>103414</v>
       </c>
@@ -26916,7 +26922,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L34" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:L34" xr:uid="{00000000-0009-0000-0000-000004000000}">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="Versaline"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" xr:uid="{8BE85DCA-83E9-4797-8D4C-27CA93E39493}"/>
   </hyperlinks>
@@ -26979,17 +26991,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr codeName="Sheet6" filterMode="1"/>
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="207.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
@@ -27051,15 +27063,15 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>136335</v>
       </c>
       <c r="B2" t="s">
         <v>1120</v>
       </c>
-      <c r="C2" t="s">
-        <v>1667</v>
+      <c r="C2" s="4" t="s">
+        <v>2031</v>
       </c>
       <c r="E2" t="s">
         <v>743</v>
@@ -27092,7 +27104,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>136679</v>
       </c>
@@ -27100,7 +27112,7 @@
         <v>1125</v>
       </c>
       <c r="C3" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="E3" t="s">
         <v>1126</v>
@@ -27133,7 +27145,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>136271</v>
       </c>
@@ -27141,7 +27153,7 @@
         <v>1132</v>
       </c>
       <c r="C4" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="E4" t="s">
         <v>642</v>
@@ -27174,7 +27186,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>135662</v>
       </c>
@@ -27182,7 +27194,7 @@
         <v>1136</v>
       </c>
       <c r="C5" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="E5" t="s">
         <v>540</v>
@@ -27215,7 +27227,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>139584</v>
       </c>
@@ -27223,7 +27235,7 @@
         <v>1139</v>
       </c>
       <c r="C6" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="E6" t="s">
         <v>536</v>
@@ -27256,7 +27268,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>105318</v>
       </c>
@@ -27264,7 +27276,7 @@
         <v>1144</v>
       </c>
       <c r="C7" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="E7" t="s">
         <v>694</v>
@@ -27297,7 +27309,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>139681</v>
       </c>
@@ -27305,7 +27317,7 @@
         <v>1149</v>
       </c>
       <c r="C8" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="E8" t="s">
         <v>510</v>
@@ -27338,7 +27350,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>138762</v>
       </c>
@@ -27346,7 +27358,7 @@
         <v>1152</v>
       </c>
       <c r="C9" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="E9" t="s">
         <v>743</v>
@@ -27387,7 +27399,7 @@
         <v>1155</v>
       </c>
       <c r="C10" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="E10" t="s">
         <v>1020</v>
@@ -27420,7 +27432,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>139349</v>
       </c>
@@ -27428,7 +27440,7 @@
         <v>1462</v>
       </c>
       <c r="C11" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="E11" t="s">
         <v>642</v>
@@ -27461,7 +27473,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>137935</v>
       </c>
@@ -27469,7 +27481,7 @@
         <v>1159</v>
       </c>
       <c r="C12" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="E12" t="s">
         <v>1154</v>
@@ -27510,7 +27522,7 @@
         <v>1162</v>
       </c>
       <c r="C13" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="E13" t="s">
         <v>645</v>
@@ -27543,7 +27555,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>135690</v>
       </c>
@@ -27551,7 +27563,7 @@
         <v>1166</v>
       </c>
       <c r="C14" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="E14" t="s">
         <v>642</v>
@@ -27592,7 +27604,7 @@
         <v>1169</v>
       </c>
       <c r="C15" t="s">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="E15" t="s">
         <v>510</v>
@@ -27633,7 +27645,7 @@
         <v>1171</v>
       </c>
       <c r="C16" t="s">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="E16" t="s">
         <v>743</v>
@@ -27666,7 +27678,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>136656</v>
       </c>
@@ -27674,7 +27686,7 @@
         <v>1172</v>
       </c>
       <c r="C17" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="E17" t="s">
         <v>645</v>
@@ -27715,7 +27727,7 @@
         <v>1175</v>
       </c>
       <c r="C18" t="s">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E18" t="s">
         <v>743</v>
@@ -27748,7 +27760,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>135241</v>
       </c>
@@ -27756,7 +27768,7 @@
         <v>1178</v>
       </c>
       <c r="C19" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="E19" t="s">
         <v>1179</v>
@@ -27789,7 +27801,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>134665</v>
       </c>
@@ -27797,7 +27809,7 @@
         <v>1184</v>
       </c>
       <c r="C20" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="E20" t="s">
         <v>1020</v>
@@ -27830,7 +27842,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>136671</v>
       </c>
@@ -27838,7 +27850,7 @@
         <v>1186</v>
       </c>
       <c r="C21" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="E21" t="s">
         <v>642</v>
@@ -27871,7 +27883,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>137835</v>
       </c>
@@ -27879,7 +27891,7 @@
         <v>1188</v>
       </c>
       <c r="C22" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="E22" t="s">
         <v>1189</v>
@@ -27912,7 +27924,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>138541</v>
       </c>
@@ -27920,7 +27932,7 @@
         <v>1192</v>
       </c>
       <c r="C23" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="E23" t="s">
         <v>486</v>
@@ -27961,7 +27973,7 @@
         <v>1195</v>
       </c>
       <c r="C24" t="s">
-        <v>1994</v>
+        <v>1992</v>
       </c>
       <c r="E24" t="s">
         <v>843</v>
@@ -27994,7 +28006,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>138954</v>
       </c>
@@ -28002,7 +28014,7 @@
         <v>1198</v>
       </c>
       <c r="C25" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="E25" t="s">
         <v>474</v>
@@ -28035,7 +28047,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>139586</v>
       </c>
@@ -28043,7 +28055,7 @@
         <v>1200</v>
       </c>
       <c r="C26" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="E26" t="s">
         <v>642</v>
@@ -28076,7 +28088,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>139578</v>
       </c>
@@ -28084,7 +28096,7 @@
         <v>1201</v>
       </c>
       <c r="C27" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="E27" t="s">
         <v>642</v>
@@ -28117,7 +28129,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>139352</v>
       </c>
@@ -28125,7 +28137,7 @@
         <v>1463</v>
       </c>
       <c r="C28" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="E28" t="s">
         <v>642</v>
@@ -28158,7 +28170,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>138521</v>
       </c>
@@ -28166,7 +28178,7 @@
         <v>1464</v>
       </c>
       <c r="C29" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="E29" t="s">
         <v>1187</v>
@@ -28199,7 +28211,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>136694</v>
       </c>
@@ -28207,7 +28219,7 @@
         <v>1205</v>
       </c>
       <c r="C30" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="E30" t="s">
         <v>743</v>
@@ -28248,7 +28260,7 @@
         <v>1207</v>
       </c>
       <c r="C31" t="s">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="E31" t="s">
         <v>1208</v>
@@ -28281,7 +28293,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>136883</v>
       </c>
@@ -28289,7 +28301,7 @@
         <v>1211</v>
       </c>
       <c r="C32" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="E32" t="s">
         <v>574</v>
@@ -28330,7 +28342,7 @@
         <v>1212</v>
       </c>
       <c r="C33" t="s">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="E33" t="s">
         <v>797</v>
@@ -28371,7 +28383,7 @@
         <v>1214</v>
       </c>
       <c r="C34" t="s">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="E34" t="s">
         <v>518</v>
@@ -28412,7 +28424,7 @@
         <v>1216</v>
       </c>
       <c r="C35" t="s">
-        <v>1998</v>
+        <v>1996</v>
       </c>
       <c r="E35" t="s">
         <v>1180</v>
@@ -28453,7 +28465,7 @@
         <v>1217</v>
       </c>
       <c r="C36" t="s">
-        <v>1999</v>
+        <v>1997</v>
       </c>
       <c r="E36" t="s">
         <v>1218</v>
@@ -28486,7 +28498,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>135672</v>
       </c>
@@ -28494,7 +28506,7 @@
         <v>1220</v>
       </c>
       <c r="C37" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="E37" t="s">
         <v>1020</v>
@@ -28527,7 +28539,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>139675</v>
       </c>
@@ -28535,7 +28547,7 @@
         <v>1221</v>
       </c>
       <c r="C38" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="E38" t="s">
         <v>1020</v>
@@ -28576,7 +28588,7 @@
         <v>1223</v>
       </c>
       <c r="C39" t="s">
-        <v>2000</v>
+        <v>1998</v>
       </c>
       <c r="E39" t="s">
         <v>1224</v>
@@ -28609,7 +28621,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>135324</v>
       </c>
@@ -28617,7 +28629,7 @@
         <v>1225</v>
       </c>
       <c r="C40" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="E40" t="s">
         <v>743</v>
@@ -28658,7 +28670,7 @@
         <v>1226</v>
       </c>
       <c r="C41" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="E41" t="s">
         <v>714</v>
@@ -28699,7 +28711,7 @@
         <v>1228</v>
       </c>
       <c r="C42" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="E42" t="s">
         <v>1219</v>
@@ -28740,7 +28752,7 @@
         <v>1230</v>
       </c>
       <c r="C43" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="E43" t="s">
         <v>1229</v>
@@ -28781,7 +28793,7 @@
         <v>1231</v>
       </c>
       <c r="C44" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="E44" t="s">
         <v>843</v>
@@ -28814,7 +28826,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>105418</v>
       </c>
@@ -28822,7 +28834,7 @@
         <v>1232</v>
       </c>
       <c r="C45" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="E45" t="s">
         <v>694</v>
@@ -28855,7 +28867,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>135242</v>
       </c>
@@ -28863,7 +28875,7 @@
         <v>1234</v>
       </c>
       <c r="C46" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="E46" t="s">
         <v>1180</v>
@@ -28896,7 +28908,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>136693</v>
       </c>
@@ -28904,7 +28916,7 @@
         <v>1235</v>
       </c>
       <c r="C47" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="E47" t="s">
         <v>642</v>
@@ -28945,7 +28957,7 @@
         <v>1237</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="E48" t="s">
         <v>1180</v>
@@ -28986,7 +28998,7 @@
         <v>1240</v>
       </c>
       <c r="C49" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="E49" t="s">
         <v>1241</v>
@@ -29019,7 +29031,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>136655</v>
       </c>
@@ -29027,7 +29039,7 @@
         <v>1242</v>
       </c>
       <c r="C50" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="E50" t="s">
         <v>1243</v>
@@ -29068,7 +29080,7 @@
         <v>1244</v>
       </c>
       <c r="C51" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="E51" t="s">
         <v>1187</v>
@@ -29101,7 +29113,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>138992</v>
       </c>
@@ -29109,7 +29121,7 @@
         <v>1245</v>
       </c>
       <c r="C52" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="E52" t="s">
         <v>474</v>
@@ -29142,7 +29154,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>135334</v>
       </c>
@@ -29150,7 +29162,7 @@
         <v>1465</v>
       </c>
       <c r="C53" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="E53" t="s">
         <v>642</v>
@@ -29191,7 +29203,7 @@
         <v>1249</v>
       </c>
       <c r="C54" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="E54" t="s">
         <v>510</v>
@@ -29224,7 +29236,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>137864</v>
       </c>
@@ -29232,7 +29244,7 @@
         <v>1250</v>
       </c>
       <c r="C55" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="E55" t="s">
         <v>1077</v>
@@ -29265,7 +29277,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>135323</v>
       </c>
@@ -29273,7 +29285,7 @@
         <v>1251</v>
       </c>
       <c r="C56" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="E56" t="s">
         <v>642</v>
@@ -29306,7 +29318,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>105417</v>
       </c>
@@ -29314,7 +29326,7 @@
         <v>1252</v>
       </c>
       <c r="C57" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="E57" t="s">
         <v>1253</v>
@@ -29347,7 +29359,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>135691</v>
       </c>
@@ -29355,7 +29367,7 @@
         <v>1254</v>
       </c>
       <c r="C58" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="E58" t="s">
         <v>743</v>
@@ -29388,7 +29400,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>135875</v>
       </c>
@@ -29396,7 +29408,7 @@
         <v>1255</v>
       </c>
       <c r="C59" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="E59" t="s">
         <v>486</v>
@@ -29437,7 +29449,7 @@
         <v>1258</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="G60" t="s">
         <v>460</v>
@@ -29464,7 +29476,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>137873</v>
       </c>
@@ -29472,7 +29484,7 @@
         <v>1261</v>
       </c>
       <c r="C61" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="E61" t="s">
         <v>886</v>
@@ -29505,7 +29517,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>135870</v>
       </c>
@@ -29513,7 +29525,7 @@
         <v>1262</v>
       </c>
       <c r="C62" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="E62" t="s">
         <v>474</v>
@@ -29554,7 +29566,7 @@
         <v>1263</v>
       </c>
       <c r="C63" t="s">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="E63" t="s">
         <v>1243</v>
@@ -29587,7 +29599,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>134664</v>
       </c>
@@ -29595,7 +29607,7 @@
         <v>1265</v>
       </c>
       <c r="C64" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="E64" t="s">
         <v>1187</v>
@@ -29636,7 +29648,7 @@
         <v>1266</v>
       </c>
       <c r="C65" t="s">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E65" t="s">
         <v>1020</v>
@@ -29677,7 +29689,7 @@
         <v>1267</v>
       </c>
       <c r="C66" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="E66" t="s">
         <v>714</v>
@@ -29710,7 +29722,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>135322</v>
       </c>
@@ -29718,7 +29730,7 @@
         <v>1225</v>
       </c>
       <c r="C67" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="E67" t="s">
         <v>743</v>
@@ -29751,7 +29763,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>138950</v>
       </c>
@@ -29759,7 +29771,7 @@
         <v>1268</v>
       </c>
       <c r="C68" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="E68" t="s">
         <v>474</v>
@@ -29792,7 +29804,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>138996</v>
       </c>
@@ -29800,7 +29812,7 @@
         <v>1269</v>
       </c>
       <c r="C69" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="E69" t="s">
         <v>474</v>
@@ -29841,7 +29853,7 @@
         <v>1272</v>
       </c>
       <c r="C70" t="s">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="E70" t="s">
         <v>510</v>
@@ -29874,7 +29886,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>138997</v>
       </c>
@@ -29882,7 +29894,7 @@
         <v>1273</v>
       </c>
       <c r="C71" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="E71" t="s">
         <v>486</v>
@@ -29915,7 +29927,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>135321</v>
       </c>
@@ -29923,7 +29935,7 @@
         <v>1251</v>
       </c>
       <c r="C72" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E72" t="s">
         <v>642</v>
@@ -29956,7 +29968,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>135335</v>
       </c>
@@ -29964,7 +29976,7 @@
         <v>1466</v>
       </c>
       <c r="C73" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="E73" t="s">
         <v>743</v>
@@ -29997,7 +30009,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>137833</v>
       </c>
@@ -30005,7 +30017,7 @@
         <v>1274</v>
       </c>
       <c r="C74" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="E74" t="s">
         <v>1275</v>
@@ -30046,7 +30058,7 @@
         <v>1276</v>
       </c>
       <c r="C75" t="s">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="E75" t="s">
         <v>1229</v>
@@ -30079,7 +30091,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>105317</v>
       </c>
@@ -30087,7 +30099,7 @@
         <v>1277</v>
       </c>
       <c r="C76" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="E76" t="s">
         <v>1253</v>
@@ -30128,7 +30140,7 @@
         <v>1278</v>
       </c>
       <c r="C77" t="s">
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="E77" t="s">
         <v>1180</v>
@@ -30161,7 +30173,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>138761</v>
       </c>
@@ -30169,7 +30181,7 @@
         <v>1279</v>
       </c>
       <c r="C78" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="E78" t="s">
         <v>510</v>
@@ -30202,7 +30214,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>138520</v>
       </c>
@@ -30210,7 +30222,7 @@
         <v>1467</v>
       </c>
       <c r="C79" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="E79" t="s">
         <v>1224</v>
@@ -30243,7 +30255,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>135665</v>
       </c>
@@ -30251,7 +30263,7 @@
         <v>1280</v>
       </c>
       <c r="C80" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="E80" t="s">
         <v>1020</v>
@@ -30284,7 +30296,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>105420</v>
       </c>
@@ -30292,7 +30304,7 @@
         <v>1281</v>
       </c>
       <c r="C81" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="E81" t="s">
         <v>1282</v>
@@ -30333,7 +30345,7 @@
         <v>1284</v>
       </c>
       <c r="C82" t="s">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="E82" t="s">
         <v>645</v>
@@ -30366,7 +30378,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>138952</v>
       </c>
@@ -30374,7 +30386,7 @@
         <v>1286</v>
       </c>
       <c r="C83" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="E83" t="s">
         <v>486</v>
@@ -30415,7 +30427,7 @@
         <v>1287</v>
       </c>
       <c r="C84" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="E84" t="s">
         <v>1020</v>
@@ -30448,7 +30460,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>138460</v>
       </c>
@@ -30456,7 +30468,7 @@
         <v>1288</v>
       </c>
       <c r="C85" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="E85" t="s">
         <v>474</v>
@@ -30497,7 +30509,7 @@
         <v>1291</v>
       </c>
       <c r="C86" t="s">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="E86" t="s">
         <v>1020</v>
@@ -30530,7 +30542,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>139579</v>
       </c>
@@ -30538,7 +30550,7 @@
         <v>1292</v>
       </c>
       <c r="C87" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="E87" t="s">
         <v>574</v>
@@ -30579,7 +30591,7 @@
         <v>1293</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="E88" t="s">
         <v>843</v>
@@ -30612,7 +30624,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>135238</v>
       </c>
@@ -30620,7 +30632,7 @@
         <v>1294</v>
       </c>
       <c r="C89" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="E89" t="s">
         <v>843</v>
@@ -30653,7 +30665,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>139580</v>
       </c>
@@ -30661,7 +30673,7 @@
         <v>1297</v>
       </c>
       <c r="C90" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="E90" t="s">
         <v>743</v>
@@ -30694,7 +30706,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>135243</v>
       </c>
@@ -30702,7 +30714,7 @@
         <v>1298</v>
       </c>
       <c r="C91" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="E91" t="s">
         <v>889</v>
@@ -30735,7 +30747,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>135244</v>
       </c>
@@ -30743,7 +30755,7 @@
         <v>1299</v>
       </c>
       <c r="C92" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="E92" t="s">
         <v>843</v>
@@ -30776,7 +30788,7 @@
         <v>1183</v>
       </c>
     </row>
-    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>139682</v>
       </c>
@@ -30784,7 +30796,7 @@
         <v>1300</v>
       </c>
       <c r="C93" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="E93" t="s">
         <v>1020</v>
@@ -30817,7 +30829,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>134572</v>
       </c>
@@ -30825,7 +30837,7 @@
         <v>1301</v>
       </c>
       <c r="C94" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="E94" t="s">
         <v>1020</v>
@@ -30866,7 +30878,7 @@
         <v>1302</v>
       </c>
       <c r="C95" t="s">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="E95" t="s">
         <v>1187</v>
@@ -30899,7 +30911,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>139587</v>
       </c>
@@ -30907,7 +30919,7 @@
         <v>1303</v>
       </c>
       <c r="C96" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="E96" t="s">
         <v>743</v>
@@ -30940,7 +30952,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>137933</v>
       </c>
@@ -30948,7 +30960,7 @@
         <v>1304</v>
       </c>
       <c r="C97" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="E97" t="s">
         <v>1078</v>
@@ -30981,7 +30993,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>139577</v>
       </c>
@@ -30989,7 +31001,7 @@
         <v>1305</v>
       </c>
       <c r="C98" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="E98" t="s">
         <v>1306</v>
@@ -31022,7 +31034,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>136615</v>
       </c>
@@ -31030,7 +31042,7 @@
         <v>1307</v>
       </c>
       <c r="C99" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="E99" t="s">
         <v>1308</v>
@@ -31063,7 +31075,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>135237</v>
       </c>
@@ -31071,7 +31083,7 @@
         <v>1310</v>
       </c>
       <c r="C100" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="E100" t="s">
         <v>889</v>
@@ -31104,7 +31116,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>135693</v>
       </c>
@@ -31112,7 +31124,7 @@
         <v>1311</v>
       </c>
       <c r="C101" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="E101" t="s">
         <v>642</v>
@@ -31145,7 +31157,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>134674</v>
       </c>
@@ -31153,7 +31165,7 @@
         <v>1312</v>
       </c>
       <c r="C102" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="E102" t="s">
         <v>510</v>
@@ -31186,7 +31198,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>139575</v>
       </c>
@@ -31194,7 +31206,7 @@
         <v>1314</v>
       </c>
       <c r="C103" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="E103" t="s">
         <v>536</v>
@@ -31227,7 +31239,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>134675</v>
       </c>
@@ -31235,7 +31247,7 @@
         <v>1315</v>
       </c>
       <c r="C104" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="E104" t="s">
         <v>1020</v>
@@ -31276,7 +31288,7 @@
         <v>1316</v>
       </c>
       <c r="C105" t="s">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="E105" t="s">
         <v>1317</v>
@@ -31317,7 +31329,7 @@
         <v>1318</v>
       </c>
       <c r="C106" t="s">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="E106" t="s">
         <v>1218</v>
@@ -31350,7 +31362,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>104180</v>
       </c>
@@ -31358,7 +31370,7 @@
         <v>1320</v>
       </c>
       <c r="C107" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="E107" t="s">
         <v>518</v>
@@ -31399,7 +31411,7 @@
         <v>1322</v>
       </c>
       <c r="C108" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="E108" t="s">
         <v>1229</v>
@@ -31432,7 +31444,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>138993</v>
       </c>
@@ -31440,7 +31452,7 @@
         <v>1323</v>
       </c>
       <c r="C109" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="E109" t="s">
         <v>486</v>
@@ -31473,7 +31485,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>134571</v>
       </c>
@@ -31481,7 +31493,7 @@
         <v>1324</v>
       </c>
       <c r="C110" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="E110" t="s">
         <v>510</v>
@@ -31514,7 +31526,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>136676</v>
       </c>
@@ -31522,7 +31534,7 @@
         <v>1325</v>
       </c>
       <c r="C111" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="E111" t="s">
         <v>536</v>
@@ -31555,7 +31567,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>137865</v>
       </c>
@@ -31563,7 +31575,7 @@
         <v>1326</v>
       </c>
       <c r="C112" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="E112" t="s">
         <v>1077</v>
@@ -31596,7 +31608,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>135332</v>
       </c>
@@ -31604,7 +31616,7 @@
         <v>1468</v>
       </c>
       <c r="C113" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="E113" t="s">
         <v>743</v>
@@ -31637,7 +31649,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>105316</v>
       </c>
@@ -31645,7 +31657,7 @@
         <v>1328</v>
       </c>
       <c r="C114" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="E114" t="s">
         <v>571</v>
@@ -31678,7 +31690,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>105419</v>
       </c>
@@ -31686,7 +31698,7 @@
         <v>1329</v>
       </c>
       <c r="C115" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="E115" t="s">
         <v>1282</v>
@@ -31719,7 +31731,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>137874</v>
       </c>
@@ -31727,7 +31739,7 @@
         <v>1330</v>
       </c>
       <c r="C116" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="E116" t="s">
         <v>886</v>
@@ -31760,7 +31772,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>137668</v>
       </c>
@@ -31768,7 +31780,7 @@
         <v>1331</v>
       </c>
       <c r="C117" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="E117" t="s">
         <v>510</v>
@@ -31801,7 +31813,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>138540</v>
       </c>
@@ -31809,7 +31821,7 @@
         <v>1332</v>
       </c>
       <c r="C118" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="E118" t="s">
         <v>474</v>
@@ -31850,7 +31862,7 @@
         <v>1333</v>
       </c>
       <c r="C119" t="s">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="E119" t="s">
         <v>1285</v>
@@ -31891,7 +31903,7 @@
         <v>1334</v>
       </c>
       <c r="C120" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="E120" t="s">
         <v>1243</v>
@@ -31924,7 +31936,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>135671</v>
       </c>
@@ -31932,7 +31944,7 @@
         <v>1335</v>
       </c>
       <c r="C121" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="E121" t="s">
         <v>510</v>
@@ -31965,7 +31977,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>138475</v>
       </c>
@@ -31973,7 +31985,7 @@
         <v>1336</v>
       </c>
       <c r="C122" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="E122" t="s">
         <v>486</v>
@@ -32014,7 +32026,7 @@
         <v>1337</v>
       </c>
       <c r="C123" t="s">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="E123" t="s">
         <v>1133</v>
@@ -32047,7 +32059,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>136690</v>
       </c>
@@ -32055,7 +32067,7 @@
         <v>1338</v>
       </c>
       <c r="C124" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="E124" t="s">
         <v>642</v>
@@ -32088,7 +32100,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>136626</v>
       </c>
@@ -32096,7 +32108,7 @@
         <v>1340</v>
       </c>
       <c r="C125" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="E125" t="s">
         <v>1219</v>
@@ -32129,7 +32141,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>135663</v>
       </c>
@@ -32137,7 +32149,7 @@
         <v>1236</v>
       </c>
       <c r="C126" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="E126" t="s">
         <v>510</v>
@@ -32170,7 +32182,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>138956</v>
       </c>
@@ -32178,7 +32190,7 @@
         <v>1342</v>
       </c>
       <c r="C127" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="E127" t="s">
         <v>486</v>
@@ -32211,7 +32223,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>136691</v>
       </c>
@@ -32219,7 +32231,7 @@
         <v>1343</v>
       </c>
       <c r="C128" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="E128" t="s">
         <v>743</v>
@@ -32252,7 +32264,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>136672</v>
       </c>
@@ -32260,7 +32272,7 @@
         <v>1344</v>
       </c>
       <c r="C129" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="E129" t="s">
         <v>743</v>
@@ -32293,7 +32305,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>135235</v>
       </c>
@@ -32301,7 +32313,7 @@
         <v>1345</v>
       </c>
       <c r="C130" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="E130" t="s">
         <v>1179</v>
@@ -32342,7 +32354,7 @@
         <v>1346</v>
       </c>
       <c r="C131" t="s">
-        <v>2003</v>
+        <v>2001</v>
       </c>
       <c r="E131" t="s">
         <v>1020</v>
@@ -32375,7 +32387,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>104181</v>
       </c>
@@ -32383,7 +32395,7 @@
         <v>1347</v>
       </c>
       <c r="C132" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="E132" t="s">
         <v>797</v>
@@ -32416,7 +32428,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>134662</v>
       </c>
@@ -32424,7 +32436,7 @@
         <v>1348</v>
       </c>
       <c r="C133" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="E133" t="s">
         <v>540</v>
@@ -32457,7 +32469,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>137836</v>
       </c>
@@ -32465,7 +32477,7 @@
         <v>1349</v>
       </c>
       <c r="C134" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="E134" t="s">
         <v>1350</v>
@@ -32498,7 +32510,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>137680</v>
       </c>
@@ -32506,7 +32518,7 @@
         <v>1351</v>
       </c>
       <c r="C135" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="E135" t="s">
         <v>1352</v>
@@ -32539,7 +32551,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>137681</v>
       </c>
@@ -32547,7 +32559,7 @@
         <v>1355</v>
       </c>
       <c r="C136" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="E136" t="s">
         <v>1356</v>
@@ -32580,7 +32592,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>139350</v>
       </c>
@@ -32588,7 +32600,7 @@
         <v>1469</v>
       </c>
       <c r="C137" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="E137" t="s">
         <v>743</v>
@@ -32621,7 +32633,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>135331</v>
       </c>
@@ -32629,7 +32641,7 @@
         <v>1470</v>
       </c>
       <c r="C138" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="E138" t="s">
         <v>642</v>
@@ -32670,7 +32682,7 @@
         <v>1357</v>
       </c>
       <c r="C139" t="s">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E139" t="s">
         <v>1127</v>
@@ -32703,7 +32715,7 @@
         <v>1210</v>
       </c>
     </row>
-    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>134562</v>
       </c>
@@ -32711,7 +32723,7 @@
         <v>1358</v>
       </c>
       <c r="C140" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="E140" t="s">
         <v>540</v>
@@ -32744,7 +32756,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>139353</v>
       </c>
@@ -32752,7 +32764,7 @@
         <v>1471</v>
       </c>
       <c r="C141" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="E141" t="s">
         <v>743</v>
@@ -32785,7 +32797,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>139576</v>
       </c>
@@ -32793,7 +32805,7 @@
         <v>1359</v>
       </c>
       <c r="C142" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="E142" t="s">
         <v>1126</v>
@@ -32826,7 +32838,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>136645</v>
       </c>
@@ -32834,7 +32846,7 @@
         <v>1360</v>
       </c>
       <c r="C143" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="E143" t="s">
         <v>714</v>
@@ -32867,7 +32879,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>135694</v>
       </c>
@@ -32875,7 +32887,7 @@
         <v>1361</v>
       </c>
       <c r="C144" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="E144" t="s">
         <v>743</v>
@@ -32908,7 +32920,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>137832</v>
       </c>
@@ -32916,7 +32928,7 @@
         <v>1362</v>
       </c>
       <c r="C145" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="E145" t="s">
         <v>670</v>
@@ -32949,7 +32961,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>136435</v>
       </c>
@@ -32957,7 +32969,7 @@
         <v>1363</v>
       </c>
       <c r="C146" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="E146" t="s">
         <v>536</v>
@@ -32990,7 +33002,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>137937</v>
       </c>
@@ -32998,7 +33010,7 @@
         <v>1364</v>
       </c>
       <c r="C147" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="E147" t="s">
         <v>1083</v>
@@ -33031,7 +33043,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>139674</v>
       </c>
@@ -33039,7 +33051,7 @@
         <v>1365</v>
       </c>
       <c r="C148" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="E148" t="s">
         <v>510</v>
@@ -33072,7 +33084,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>136605</v>
       </c>
@@ -33080,7 +33092,7 @@
         <v>1366</v>
       </c>
       <c r="C149" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="E149" t="s">
         <v>1367</v>
@@ -33121,7 +33133,7 @@
         <v>1369</v>
       </c>
       <c r="C150" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="E150" t="s">
         <v>642</v>
@@ -33154,7 +33166,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>136677</v>
       </c>
@@ -33162,7 +33174,7 @@
         <v>1370</v>
       </c>
       <c r="C151" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="E151" t="s">
         <v>1306</v>
@@ -33195,7 +33207,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>137863</v>
       </c>
@@ -33203,7 +33215,7 @@
         <v>1371</v>
       </c>
       <c r="C152" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="E152" t="s">
         <v>1077</v>
@@ -33236,7 +33248,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>138470</v>
       </c>
@@ -33244,7 +33256,7 @@
         <v>1336</v>
       </c>
       <c r="C153" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="E153" t="s">
         <v>486</v>
@@ -33277,7 +33289,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>138465</v>
       </c>
@@ -33285,7 +33297,7 @@
         <v>1288</v>
       </c>
       <c r="C154" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="E154" t="s">
         <v>474</v>
@@ -33318,7 +33330,7 @@
         <v>1290</v>
       </c>
     </row>
-    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>105416</v>
       </c>
@@ -33326,7 +33338,7 @@
         <v>1372</v>
       </c>
       <c r="C155" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="E155" t="s">
         <v>571</v>
@@ -33359,7 +33371,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>134663</v>
       </c>
@@ -33367,7 +33379,7 @@
         <v>1373</v>
       </c>
       <c r="C156" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="E156" t="s">
         <v>510</v>
@@ -33408,7 +33420,7 @@
         <v>1374</v>
       </c>
       <c r="C157" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E157" t="s">
         <v>1187</v>
@@ -33441,7 +33453,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>135236</v>
       </c>
@@ -33449,7 +33461,7 @@
         <v>1375</v>
       </c>
       <c r="C158" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="E158" t="s">
         <v>1180</v>
@@ -33483,49 +33495,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O158" xr:uid="{00000000-0009-0000-0000-000006000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/t_square/v1686671954/abg-graphics/original-images/maax/retail/retail/doors/aura/aura-6mm/jpeg/aura6-60-900-340-olympia.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/t_square/v1741957591/abg-graphics/original-images/maax/multi-brand/doors/kameleon/6-8-mm/jpeg/maax-kameleon-47w-shower-door-rs739-fluted-db.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/t_square/v1741957958/abg-graphics/original-images/maax/retail/home-depot-exclusives/doors/tonik/maax-tonik-47w-shower-door-rs738-fluted-db.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1633110401/abg-graphics/e-commerce/barracuda-pin-connect/duel/duel-sh60-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663272804/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-49-51x68-mb-square-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663272831/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-57-59x68-ch-round-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663272840/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-57-59x68-mb-round-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663272956/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-square-handle-bn-zoom.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273001/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-43-45x68-mb-square-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273033/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-49-51x68-bn-round-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273080/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-43-45x68-bn-round-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273167/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-27-29x68-mb-round-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273186/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-27-29x68-bn-square-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273191/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-31-33x68-bn-square-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273202/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-31-33x68-ch-round-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1663273249/abg-graphics/original-images/maax/multi-brand/doors/manhattan/jpeg/maax-manhattan-37-39x68-ch-round-handle-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1667593848/abg-graphics/original-images/maax/multi-brand/doors/uptown-pivot/jpeg/mixed-finish/uptown-pivot-sh60-db-bm-generic-walls-olympia-base.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1667593855/abg-graphics/original-images/maax/multi-brand/doors/uptown-pivot/jpeg/mixed-finish/uptown-pivot-sh48-mb-wd-u-carrara-olympia-base.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1675700017/abg-graphics/original-images/maax/multi-brand/doors/duel-alto/jpeg/4836-duel-alto-bn-mb-utile-tosca-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1675700022/abg-graphics/original-images/maax/multi-brand/doors/duel-alto/jpeg/6036-duel-alto-ch-mw-utile-tosca.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1686671954/abg-graphics/original-images/maax/retail/retail/doors/aura/aura-6mm/jpeg/aura6-60-900-340-olympia.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1686673218/abg-graphics/original-images/maax/retail/retail/doors/aura/aura-8mm/jpeg/aura8-60-900-340-olympia.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1686673630/abg-graphics/original-images/maax/retail/retail/doors/aura/aura-8mm/jpeg/aura8-48-900-340-b3square.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1686675109/abg-graphics/original-images/maax/multi-brand/doors/kameleon/6-8-mm/jpeg/kameleon-60-900-340.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1692029122/abg-graphics/original-images/maax/multi-brand/doors/polar-shower/jpeg/maax-polar48-bypass-ch-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1692029126/abg-graphics/original-images/maax/multi-brand/doors/polar-shower/jpeg/maax-polar60-bypass-ch-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1692029242/abg-graphics/original-images/maax/multi-brand/doors/polar-pivot/maax-polar-pivot-27-29-ch-1.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1692029243/abg-graphics/original-images/maax/multi-brand/doors/polar-pivot/maax-polar-pivot-33-35-ch-2.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1726861944/abg-graphics/original-images/maax/multi-brand/doors/pivolok/jpeg/maax-pivolok-23-ch-raindrop-close-pano.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1726861957/abg-graphics/original-images/maax/multi-brand/doors/pivolok/jpeg/maax-pivolok-27-ch-raindrop-close-pano.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/v1737472895/abg-graphics/original-images/maax/multi-brand/doors/kameleon/6-8-mm/jpeg/kameleon-60-978-340.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/w_1500,h_1260,c_fill/v1660858069/abg-graphics/original-images/maax/multi-brand/doors/odyssey/jpeg/maax-48-odyssey-mb-u-tux-zone-deco.jpg"/>
-        <filter val="https://res.cloudinary.com/american-bath-group/image/upload/c_crop,w_1260,h_1260/w_1500,h_1260,c_fill/v1664220622/abg-graphics/original-images/maax/multi-brand/doors/odyssey/jpeg/maax-odyssey-sh-60-ch-zone-base-deco.jpg"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O158" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <hyperlinks>
     <hyperlink ref="C48" r:id="rId1" xr:uid="{418F516E-2E2B-49D8-B66A-753E68587D51}"/>
     <hyperlink ref="C60" r:id="rId2" xr:uid="{33E723EC-4207-4B4C-A8F7-92003E66D403}"/>
     <hyperlink ref="C88" r:id="rId3" xr:uid="{AF157174-0343-42AB-A9D7-EB44DFB48C3C}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{9734DA33-E16A-4B61-88CA-6880FF72E9EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33535,8 +33510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33600,7 +33575,7 @@
         <v>1380</v>
       </c>
       <c r="C2" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="E2" t="s">
         <v>486</v>
@@ -33635,7 +33610,7 @@
         <v>1402</v>
       </c>
       <c r="C3" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="E3" t="s">
         <v>1187</v>
@@ -33670,7 +33645,7 @@
         <v>1455</v>
       </c>
       <c r="C4" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="E4" t="s">
         <v>743</v>
@@ -33705,7 +33680,7 @@
         <v>1456</v>
       </c>
       <c r="C5" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="E5" t="s">
         <v>743</v>
@@ -33740,7 +33715,7 @@
         <v>1457</v>
       </c>
       <c r="C6" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="E6" t="s">
         <v>743</v>
@@ -33775,7 +33750,7 @@
         <v>1400</v>
       </c>
       <c r="C7" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="E7" t="s">
         <v>743</v>
@@ -33810,7 +33785,7 @@
         <v>1377</v>
       </c>
       <c r="C8" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="E8" t="s">
         <v>743</v>
@@ -33845,7 +33820,7 @@
         <v>1407</v>
       </c>
       <c r="C9" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="E9" t="s">
         <v>743</v>
@@ -33880,7 +33855,7 @@
         <v>1410</v>
       </c>
       <c r="C10" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="E10" t="s">
         <v>743</v>
@@ -33915,7 +33890,7 @@
         <v>1408</v>
       </c>
       <c r="C11" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="E11" t="s">
         <v>743</v>
@@ -33950,7 +33925,7 @@
         <v>1401</v>
       </c>
       <c r="C12" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="E12" t="s">
         <v>889</v>
@@ -33985,7 +33960,7 @@
         <v>1404</v>
       </c>
       <c r="C13" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="E13" t="s">
         <v>843</v>
@@ -34019,8 +33994,8 @@
       <c r="B14" t="s">
         <v>1386</v>
       </c>
-      <c r="C14" t="s">
-        <v>1842</v>
+      <c r="C14" s="4" t="s">
+        <v>2032</v>
       </c>
       <c r="E14" t="s">
         <v>743</v>
@@ -34055,7 +34030,7 @@
         <v>1379</v>
       </c>
       <c r="C15" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="E15" t="s">
         <v>743</v>
@@ -34090,7 +34065,7 @@
         <v>1390</v>
       </c>
       <c r="C16" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="E16" t="s">
         <v>486</v>
@@ -34125,7 +34100,7 @@
         <v>1390</v>
       </c>
       <c r="C17" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="E17" t="s">
         <v>486</v>
@@ -34160,7 +34135,7 @@
         <v>1388</v>
       </c>
       <c r="C18" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="E18" t="s">
         <v>1356</v>
@@ -34195,7 +34170,7 @@
         <v>1389</v>
       </c>
       <c r="C19" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="E19" t="s">
         <v>1187</v>
@@ -34230,7 +34205,7 @@
         <v>1381</v>
       </c>
       <c r="C20" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="E20" t="s">
         <v>1020</v>
@@ -34265,7 +34240,7 @@
         <v>1397</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="E21" t="s">
         <v>1020</v>
@@ -34300,7 +34275,7 @@
         <v>1383</v>
       </c>
       <c r="C22" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="E22" t="s">
         <v>1187</v>
@@ -34335,7 +34310,7 @@
         <v>1411</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="E23" t="s">
         <v>1020</v>
@@ -34370,7 +34345,7 @@
         <v>1393</v>
       </c>
       <c r="C24" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="E24" t="s">
         <v>1020</v>
@@ -34405,7 +34380,7 @@
         <v>1394</v>
       </c>
       <c r="C25" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="E25" t="s">
         <v>1020</v>
@@ -34440,7 +34415,7 @@
         <v>1396</v>
       </c>
       <c r="C26" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="E26" t="s">
         <v>1020</v>
@@ -34475,7 +34450,7 @@
         <v>1382</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="E27" t="s">
         <v>1020</v>
@@ -34510,7 +34485,7 @@
         <v>1399</v>
       </c>
       <c r="C28" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="E28" t="s">
         <v>1020</v>
@@ -34545,7 +34520,7 @@
         <v>1458</v>
       </c>
       <c r="C29" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="E29" t="s">
         <v>486</v>
@@ -34580,7 +34555,7 @@
         <v>1392</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>2024</v>
+        <v>2022</v>
       </c>
       <c r="E30" t="s">
         <v>1020</v>
@@ -34615,7 +34590,7 @@
         <v>1387</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E31" t="s">
         <v>1187</v>
@@ -34650,7 +34625,7 @@
         <v>1391</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="E32" t="s">
         <v>1020</v>
@@ -34685,7 +34660,7 @@
         <v>1384</v>
       </c>
       <c r="C33" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="E33" t="s">
         <v>1020</v>
@@ -34720,7 +34695,7 @@
         <v>1398</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="E34" t="s">
         <v>1020</v>
@@ -34755,7 +34730,7 @@
         <v>1266</v>
       </c>
       <c r="C35" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="E35" t="s">
         <v>1020</v>
@@ -34790,7 +34765,7 @@
         <v>1409</v>
       </c>
       <c r="C36" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="E36" t="s">
         <v>518</v>
@@ -34831,6 +34806,7 @@
     <hyperlink ref="C31" r:id="rId5" xr:uid="{0BF79A74-19E7-4BD8-A0DB-61D3791D9A27}"/>
     <hyperlink ref="C32" r:id="rId6" xr:uid="{4B546625-828B-4B64-B388-642AACE3CA64}"/>
     <hyperlink ref="C34" r:id="rId7" xr:uid="{721B6A6C-E85C-4B4A-8E78-29F4419ACDA3}"/>
+    <hyperlink ref="C14" r:id="rId8" xr:uid="{CD7B4AE1-8458-4753-A90B-C8F00DA00D48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34900,7 +34876,7 @@
         <v>1414</v>
       </c>
       <c r="C2" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D2" t="s">
         <v>43</v>
@@ -34938,7 +34914,7 @@
         <v>1461</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>2027</v>
+        <v>2025</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -34976,7 +34952,7 @@
         <v>1416</v>
       </c>
       <c r="C4" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
@@ -35014,7 +34990,7 @@
         <v>1417</v>
       </c>
       <c r="C5" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D5" t="s">
         <v>249</v>
@@ -35052,7 +35028,7 @@
         <v>1460</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>2028</v>
+        <v>2026</v>
       </c>
       <c r="D6" t="s">
         <v>249</v>
@@ -35090,7 +35066,7 @@
         <v>1419</v>
       </c>
       <c r="C7" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D7" t="s">
         <v>35</v>
@@ -35128,7 +35104,7 @@
         <v>1420</v>
       </c>
       <c r="C8" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="D8" t="s">
         <v>39</v>
@@ -35166,7 +35142,7 @@
         <v>1421</v>
       </c>
       <c r="C9" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D9" t="s">
         <v>249</v>
@@ -35204,7 +35180,7 @@
         <v>1459</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>2029</v>
+        <v>2027</v>
       </c>
       <c r="D10" t="s">
         <v>39</v>
@@ -35242,7 +35218,7 @@
         <v>1422</v>
       </c>
       <c r="C11" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="D11" t="s">
         <v>35</v>
@@ -35280,7 +35256,7 @@
         <v>1423</v>
       </c>
       <c r="C12" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D12" t="s">
         <v>39</v>

</xml_diff>